<commit_message>
Updated for switch between JH and ECDC data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81372F95-50E0-574D-AAE1-C42F5E3133B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EDC9ABC-0F8A-9841-9630-CEBA87721A92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1313" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="111">
   <si>
     <t>Date</t>
   </si>
@@ -1252,13 +1252,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K29"/>
+  <dimension ref="A1:K30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
+      <selection pane="bottomRight" activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2285,6 +2285,40 @@
       </c>
       <c r="K29" t="s">
         <v>110</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B30" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C30" s="5">
+        <v>5709</v>
+      </c>
+      <c r="D30" s="5">
+        <f>C30-C29</f>
+        <v>345</v>
+      </c>
+      <c r="E30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="5">
+        <f>36+G29</f>
+        <v>210</v>
+      </c>
+      <c r="H30" t="s">
+        <v>8</v>
+      </c>
+      <c r="I30" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected mistake in latest data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C26E45-1F4F-CF40-BBC2-6C0611AEB50C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DD09F9-6154-6646-8873-26F6E4178D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -7508,8 +7508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77735C93-7ED9-C044-B61C-E23C86F44D03}">
   <dimension ref="A1:E541"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A505" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="B516" sqref="B516"/>
+    <sheetView tabSelected="1" topLeftCell="A502" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A512" sqref="A512"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15232,7 +15232,7 @@
     </row>
     <row r="517" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A517" s="1">
-        <v>43927</v>
+        <v>43926</v>
       </c>
       <c r="B517" t="s">
         <v>14</v>
@@ -15246,7 +15246,7 @@
     </row>
     <row r="518" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A518" s="1">
-        <v>43928</v>
+        <v>43926</v>
       </c>
       <c r="B518" t="s">
         <v>15</v>
@@ -15260,7 +15260,7 @@
     </row>
     <row r="519" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A519" s="1">
-        <v>43929</v>
+        <v>43926</v>
       </c>
       <c r="B519" t="s">
         <v>16</v>
@@ -15274,7 +15274,7 @@
     </row>
     <row r="520" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A520" s="1">
-        <v>43930</v>
+        <v>43926</v>
       </c>
       <c r="B520" t="s">
         <v>17</v>
@@ -15288,7 +15288,7 @@
     </row>
     <row r="521" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A521" s="1">
-        <v>43931</v>
+        <v>43926</v>
       </c>
       <c r="B521" t="s">
         <v>18</v>
@@ -15302,7 +15302,7 @@
     </row>
     <row r="522" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A522" s="1">
-        <v>43932</v>
+        <v>43926</v>
       </c>
       <c r="B522" t="s">
         <v>19</v>
@@ -15316,7 +15316,7 @@
     </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A523" s="1">
-        <v>43933</v>
+        <v>43926</v>
       </c>
       <c r="B523" t="s">
         <v>20</v>
@@ -15330,7 +15330,7 @@
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A524" s="1">
-        <v>43934</v>
+        <v>43926</v>
       </c>
       <c r="B524" t="s">
         <v>21</v>
@@ -15344,7 +15344,7 @@
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A525" s="1">
-        <v>43935</v>
+        <v>43926</v>
       </c>
       <c r="B525" t="s">
         <v>22</v>
@@ -15358,7 +15358,7 @@
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A526" s="1">
-        <v>43936</v>
+        <v>43926</v>
       </c>
       <c r="B526" t="s">
         <v>36</v>
@@ -15372,7 +15372,7 @@
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A527" s="1">
-        <v>43937</v>
+        <v>43926</v>
       </c>
       <c r="B527" t="s">
         <v>37</v>
@@ -15386,7 +15386,7 @@
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A528" s="1">
-        <v>43938</v>
+        <v>43926</v>
       </c>
       <c r="B528" t="s">
         <v>23</v>
@@ -15400,7 +15400,7 @@
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A529" s="1">
-        <v>43939</v>
+        <v>43926</v>
       </c>
       <c r="B529" t="s">
         <v>24</v>
@@ -15414,7 +15414,7 @@
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A530" s="1">
-        <v>43940</v>
+        <v>43926</v>
       </c>
       <c r="B530" t="s">
         <v>25</v>
@@ -15428,7 +15428,7 @@
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A531" s="1">
-        <v>43941</v>
+        <v>43926</v>
       </c>
       <c r="B531" t="s">
         <v>26</v>
@@ -15442,7 +15442,7 @@
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A532" s="1">
-        <v>43942</v>
+        <v>43926</v>
       </c>
       <c r="B532" t="s">
         <v>27</v>
@@ -15456,7 +15456,7 @@
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A533" s="1">
-        <v>43943</v>
+        <v>43926</v>
       </c>
       <c r="B533" t="s">
         <v>38</v>
@@ -15470,7 +15470,7 @@
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A534" s="1">
-        <v>43944</v>
+        <v>43926</v>
       </c>
       <c r="B534" t="s">
         <v>28</v>
@@ -15484,7 +15484,7 @@
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A535" s="1">
-        <v>43945</v>
+        <v>43926</v>
       </c>
       <c r="B535" t="s">
         <v>29</v>
@@ -15498,7 +15498,7 @@
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A536" s="1">
-        <v>43946</v>
+        <v>43926</v>
       </c>
       <c r="B536" t="s">
         <v>30</v>
@@ -15512,7 +15512,7 @@
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A537" s="1">
-        <v>43947</v>
+        <v>43926</v>
       </c>
       <c r="B537" t="s">
         <v>31</v>
@@ -15526,7 +15526,7 @@
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A538" s="1">
-        <v>43948</v>
+        <v>43926</v>
       </c>
       <c r="B538" t="s">
         <v>32</v>
@@ -15540,7 +15540,7 @@
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A539" s="1">
-        <v>43949</v>
+        <v>43926</v>
       </c>
       <c r="B539" t="s">
         <v>33</v>
@@ -15554,7 +15554,7 @@
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A540" s="1">
-        <v>43950</v>
+        <v>43926</v>
       </c>
       <c r="B540" t="s">
         <v>34</v>
@@ -15568,7 +15568,7 @@
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A541" s="1">
-        <v>43951</v>
+        <v>43926</v>
       </c>
       <c r="B541" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
Updated latest Irish data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0DD09F9-6154-6646-8873-26F6E4178D93}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F565BEB2-F837-824B-9164-71F79658D747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1424" uniqueCount="118">
   <si>
     <t>Date</t>
   </si>
@@ -364,9 +364,6 @@
     <t>https://www.gov.ie/en/publication/ed3cdd-an-analysis-of-the-4916-cases-of-covid-19-in-ireland-as-of-saturday-/</t>
   </si>
   <si>
-    <t>https://www.gov.ie/en/press-release/ec2aa4-statement-from-the-national-public-health-emergency-team-monday-6-ap/</t>
-  </si>
-  <si>
     <t>https://www.gov.ie/en/press-release/ee6b84-statement-from-the-national-public-health-emergency-team-tuesday-7-a/</t>
   </si>
   <si>
@@ -389,6 +386,9 @@
   </si>
   <si>
     <t>677</t>
+  </si>
+  <si>
+    <t>https://www.gov.ie/en/press-release/0f1615-statement-from-the-national-public-health-emergency-team-wednesday-8/</t>
   </si>
 </sst>
 </file>
@@ -872,7 +872,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -884,6 +884,7 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1242,7 +1243,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1260,10 +1261,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43925</v>
+        <v>43926</v>
       </c>
       <c r="B2" s="1">
-        <v>43927</v>
+        <v>43929</v>
       </c>
     </row>
   </sheetData>
@@ -1273,13 +1274,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K30"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B5" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K28" sqref="K28"/>
+      <selection pane="bottomRight" activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2269,7 +2270,7 @@
         <v>48</v>
       </c>
       <c r="K28" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -2280,32 +2281,32 @@
         <v>104</v>
       </c>
       <c r="C29" s="5">
-        <v>5364</v>
+        <v>5981</v>
       </c>
       <c r="D29" s="5">
         <f>C29-C28</f>
-        <v>-229</v>
-      </c>
-      <c r="E29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>8</v>
+        <v>388</v>
+      </c>
+      <c r="E29" s="5">
+        <v>1472</v>
+      </c>
+      <c r="F29" s="5">
+        <v>224</v>
       </c>
       <c r="G29" s="5">
-        <v>174</v>
-      </c>
-      <c r="H29" t="s">
-        <v>8</v>
-      </c>
-      <c r="I29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>8</v>
+        <v>223</v>
+      </c>
+      <c r="H29">
+        <v>1568</v>
+      </c>
+      <c r="I29" s="5">
+        <v>299</v>
+      </c>
+      <c r="J29" s="5">
+        <v>48</v>
       </c>
       <c r="K29" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -2320,7 +2321,7 @@
       </c>
       <c r="D30" s="5">
         <f>C30-C29</f>
-        <v>345</v>
+        <v>-272</v>
       </c>
       <c r="E30" s="5" t="s">
         <v>8</v>
@@ -2329,7 +2330,6 @@
         <v>8</v>
       </c>
       <c r="G30" s="5">
-        <f>36+G29</f>
         <v>210</v>
       </c>
       <c r="H30" t="s">
@@ -2342,7 +2342,43 @@
         <v>8</v>
       </c>
       <c r="K30" t="s">
-        <v>110</v>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B31" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C31" s="5">
+        <v>6074</v>
+      </c>
+      <c r="D31" s="5">
+        <f>C31-C30</f>
+        <v>365</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="5">
+        <v>235</v>
+      </c>
+      <c r="H31" t="s">
+        <v>8</v>
+      </c>
+      <c r="I31" t="s">
+        <v>8</v>
+      </c>
+      <c r="J31" t="s">
+        <v>8</v>
+      </c>
+      <c r="K31" t="s">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
@@ -2352,10 +2388,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B646AB9-6DFD-6342-9B5D-CA852E35631D}">
-  <dimension ref="A1:D59"/>
+  <dimension ref="A1:D62"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D60" sqref="D60"/>
+      <selection activeCell="A60" sqref="A60:A62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3189,6 +3225,48 @@
         <v>0</v>
       </c>
     </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B60" t="s">
+        <v>61</v>
+      </c>
+      <c r="C60">
+        <v>3154</v>
+      </c>
+      <c r="D60">
+        <v>52.7</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B61" t="s">
+        <v>62</v>
+      </c>
+      <c r="C61">
+        <v>2757</v>
+      </c>
+      <c r="D61">
+        <v>46.1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62">
+        <v>70</v>
+      </c>
+      <c r="D62">
+        <v>1.2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3196,11 +3274,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2CC04-F5BC-6741-A3F2-2661873C87D7}">
-  <dimension ref="A1:D226"/>
+  <dimension ref="A1:E237"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A183" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C227" sqref="C227"/>
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D231" sqref="D231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6258,7 +6336,7 @@
         <v>8</v>
       </c>
       <c r="D218" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="219" spans="1:4" x14ac:dyDescent="0.2">
@@ -6272,7 +6350,7 @@
         <v>39</v>
       </c>
       <c r="D219" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="220" spans="1:4" x14ac:dyDescent="0.2">
@@ -6286,7 +6364,7 @@
         <v>347</v>
       </c>
       <c r="D220" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="221" spans="1:4" x14ac:dyDescent="0.2">
@@ -6314,7 +6392,7 @@
         <v>1044</v>
       </c>
       <c r="D222" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="223" spans="1:4" x14ac:dyDescent="0.2">
@@ -6328,7 +6406,7 @@
         <v>1048</v>
       </c>
       <c r="D223" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="224" spans="1:4" x14ac:dyDescent="0.2">
@@ -6342,10 +6420,10 @@
         <v>794</v>
       </c>
       <c r="D224" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.2">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
         <v>43926</v>
       </c>
@@ -6356,10 +6434,10 @@
         <v>1326</v>
       </c>
       <c r="D225" s="4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.2">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>43926</v>
       </c>
@@ -6371,6 +6449,161 @@
       </c>
       <c r="D226" s="4" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C227">
+        <v>12</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C228">
+        <v>18</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E228" s="7"/>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A229" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C229" t="s">
+        <v>8</v>
+      </c>
+      <c r="D229">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A230" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C230">
+        <v>42</v>
+      </c>
+      <c r="D230">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A231" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C231">
+        <v>364</v>
+      </c>
+      <c r="D231">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A232" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C232">
+        <v>1010</v>
+      </c>
+      <c r="D232">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A233" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B233" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C233">
+        <v>1111</v>
+      </c>
+      <c r="D233">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A234" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B234" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C234">
+        <v>1118</v>
+      </c>
+      <c r="D234">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A235" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B235" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C235">
+        <v>847</v>
+      </c>
+      <c r="D235">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B236" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C236">
+        <v>1442</v>
+      </c>
+      <c r="D236">
+        <v>739</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B237" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C237">
+        <v>17</v>
+      </c>
+      <c r="D237">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -6380,11 +6613,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029AF1D0-4AE1-A540-B628-AF7C84CE0F40}">
-  <dimension ref="A1:D79"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79:D82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7499,6 +7732,48 @@
         <v>106</v>
       </c>
     </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B80" t="s">
+        <v>56</v>
+      </c>
+      <c r="C80">
+        <v>67</v>
+      </c>
+      <c r="D80" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B81" t="s">
+        <v>57</v>
+      </c>
+      <c r="C81">
+        <v>23</v>
+      </c>
+      <c r="D81" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B82" t="s">
+        <v>58</v>
+      </c>
+      <c r="C82">
+        <v>10</v>
+      </c>
+      <c r="D82" t="s">
+        <v>106</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7506,10 +7781,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77735C93-7ED9-C044-B61C-E23C86F44D03}">
-  <dimension ref="A1:E541"/>
+  <dimension ref="A1:E567"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A502" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A512" sqref="A512"/>
+    <sheetView topLeftCell="A533" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A542" sqref="A542:A567"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -15580,6 +15855,370 @@
         <v>3.1E-2</v>
       </c>
     </row>
+    <row r="542" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A542" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B542" t="s">
+        <v>12</v>
+      </c>
+      <c r="C542">
+        <v>15</v>
+      </c>
+      <c r="D542" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="543" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A543" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B543" t="s">
+        <v>14</v>
+      </c>
+      <c r="C543">
+        <v>129</v>
+      </c>
+      <c r="D543" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="544" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A544" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B544" t="s">
+        <v>15</v>
+      </c>
+      <c r="C544">
+        <v>66</v>
+      </c>
+      <c r="D544" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="545" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A545" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B545" t="s">
+        <v>16</v>
+      </c>
+      <c r="C545">
+        <v>431</v>
+      </c>
+      <c r="D545" s="3">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="546" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A546" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B546" t="s">
+        <v>17</v>
+      </c>
+      <c r="C546">
+        <v>120</v>
+      </c>
+      <c r="D546" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="547" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A547" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B547" t="s">
+        <v>18</v>
+      </c>
+      <c r="C547">
+        <v>3268</v>
+      </c>
+      <c r="D547" s="3">
+        <v>0.54600000000000004</v>
+      </c>
+    </row>
+    <row r="548" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A548" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B548" t="s">
+        <v>19</v>
+      </c>
+      <c r="C548">
+        <v>134</v>
+      </c>
+      <c r="D548" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="549" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A549" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B549" t="s">
+        <v>20</v>
+      </c>
+      <c r="C549">
+        <v>122</v>
+      </c>
+      <c r="D549" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="550" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A550" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B550" t="s">
+        <v>21</v>
+      </c>
+      <c r="C550">
+        <v>233</v>
+      </c>
+      <c r="D550" s="3">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="551" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A551" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B551" t="s">
+        <v>22</v>
+      </c>
+      <c r="C551">
+        <v>88</v>
+      </c>
+      <c r="D551" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="552" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A552" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B552" t="s">
+        <v>36</v>
+      </c>
+      <c r="C552">
+        <v>34</v>
+      </c>
+      <c r="D552" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="553" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A553" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B553" t="s">
+        <v>37</v>
+      </c>
+      <c r="C553">
+        <v>20</v>
+      </c>
+      <c r="D553" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="554" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A554" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B554" t="s">
+        <v>23</v>
+      </c>
+      <c r="C554">
+        <v>160</v>
+      </c>
+      <c r="D554" s="3">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="555" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A555" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B555" t="s">
+        <v>24</v>
+      </c>
+      <c r="C555">
+        <v>35</v>
+      </c>
+      <c r="D555" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="556" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A556" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B556" t="s">
+        <v>25</v>
+      </c>
+      <c r="C556">
+        <v>96</v>
+      </c>
+      <c r="D556" s="3">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="557" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A557" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B557" t="s">
+        <v>26</v>
+      </c>
+      <c r="C557">
+        <v>130</v>
+      </c>
+      <c r="D557" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="558" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A558" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B558" t="s">
+        <v>27</v>
+      </c>
+      <c r="C558">
+        <v>183</v>
+      </c>
+      <c r="D558" s="3">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="559" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A559" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B559" t="s">
+        <v>38</v>
+      </c>
+      <c r="C559">
+        <v>62</v>
+      </c>
+      <c r="D559" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="560" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A560" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B560" t="s">
+        <v>28</v>
+      </c>
+      <c r="C560">
+        <v>77</v>
+      </c>
+      <c r="D560" s="3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="561" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A561" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B561" t="s">
+        <v>29</v>
+      </c>
+      <c r="C561">
+        <v>22</v>
+      </c>
+      <c r="D561" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="562" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A562" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B562" t="s">
+        <v>30</v>
+      </c>
+      <c r="C562">
+        <v>28</v>
+      </c>
+      <c r="D562" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="563" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A563" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B563" t="s">
+        <v>31</v>
+      </c>
+      <c r="C563">
+        <v>137</v>
+      </c>
+      <c r="D563" s="3">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="564" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A564" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B564" t="s">
+        <v>32</v>
+      </c>
+      <c r="C564">
+        <v>52</v>
+      </c>
+      <c r="D564" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="565" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A565" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B565" t="s">
+        <v>33</v>
+      </c>
+      <c r="C565">
+        <v>134</v>
+      </c>
+      <c r="D565" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="566" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A566" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B566" t="s">
+        <v>34</v>
+      </c>
+      <c r="C566">
+        <v>24</v>
+      </c>
+      <c r="D566" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="567" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A567" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B567" t="s">
+        <v>35</v>
+      </c>
+      <c r="C567">
+        <v>181</v>
+      </c>
+      <c r="D567" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added in sources and credits
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B32A9AC-6E70-B04D-A785-6458D29801AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D03B5D-6AD4-5742-BBB5-EA6670A4020A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1568" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="148">
   <si>
     <t>Date</t>
   </si>
@@ -481,6 +481,9 @@
   </si>
   <si>
     <t>Derry</t>
+  </si>
+  <si>
+    <t>Pos_prop</t>
   </si>
 </sst>
 </file>
@@ -927,7 +930,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -970,8 +973,9 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -986,8 +990,9 @@
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -1027,6 +1032,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Per cent" xfId="42" builtinId="5"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
@@ -1377,7 +1383,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39AE50F-07C0-7048-95B5-0C81D93B81F0}">
   <dimension ref="A1:C67"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -2255,7 +2261,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3217,7 +3223,7 @@
         <v>43926</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="5">
         <v>5593</v>
@@ -3253,7 +3259,7 @@
         <v>43927</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C29" s="5">
         <v>5981</v>
@@ -17201,15 +17207,18 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE73A96-9009-C14A-A4D6-627BDCEBA7A8}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -17228,8 +17237,11 @@
       <c r="F1" t="s">
         <v>139</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>43929</v>
       </c>
@@ -17248,8 +17260,12 @@
       <c r="F2">
         <v>9564</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G2" s="10">
+        <f>D2/F2</f>
+        <v>0.14000418235048098</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43928</v>
       </c>
@@ -17268,8 +17284,12 @@
       <c r="F3">
         <v>9158</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G9" si="0">D3/F3</f>
+        <v>0.13703865472810658</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>43927</v>
       </c>
@@ -17288,8 +17308,12 @@
       <c r="F4">
         <v>8740</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G4" s="10">
+        <f t="shared" si="0"/>
+        <v>0.13249427917620138</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>43926</v>
       </c>
@@ -17308,8 +17332,12 @@
       <c r="F5">
         <v>8486</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G5" s="10">
+        <f t="shared" si="0"/>
+        <v>0.12832901249116191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>43925</v>
       </c>
@@ -17328,8 +17356,12 @@
       <c r="F6">
         <v>8034</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G6" s="10">
+        <f t="shared" si="0"/>
+        <v>0.12422205626089121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>43924</v>
       </c>
@@ -17348,8 +17380,12 @@
       <c r="F7">
         <v>7525</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G7" s="10">
+        <f t="shared" si="0"/>
+        <v>0.12013289036544851</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>43923</v>
       </c>
@@ -17368,8 +17404,12 @@
       <c r="F8">
         <v>6899</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G8" s="10">
+        <f t="shared" si="0"/>
+        <v>0.11219017248876649</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>43922</v>
       </c>
@@ -17387,6 +17427,10 @@
       </c>
       <c r="F9">
         <v>6450</v>
+      </c>
+      <c r="G9" s="10">
+        <f t="shared" si="0"/>
+        <v>0.10682170542635659</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to latest Irish data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0D03B5D-6AD4-5742-BBB5-EA6670A4020A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042095B-0D0E-174B-AA69-55CBA3FCD603}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1569" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1635" uniqueCount="150">
   <si>
     <t>Date</t>
   </si>
@@ -484,6 +484,12 @@
   </si>
   <si>
     <t>Pos_prop</t>
+  </si>
+  <si>
+    <t>https://www.gov.ie/en/news/7e0924-latest-updates-on-covid-19-coronavirus/#april-9</t>
+  </si>
+  <si>
+    <t>https://www.gov.ie/en/publication/695f10-an-analysis-of-the-6444-cases-of-covid-19-in-ireland-as-of-tuesday-7/</t>
   </si>
 </sst>
 </file>
@@ -975,7 +981,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -991,6 +997,7 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1381,13 +1388,17 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39AE50F-07C0-7048-95B5-0C81D93B81F0}">
-  <dimension ref="A1:C67"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
@@ -1405,10 +1416,10 @@
         <v>118</v>
       </c>
       <c r="B2" s="8">
-        <v>81</v>
+        <v>89</v>
       </c>
       <c r="C2" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1416,10 +1427,10 @@
         <v>119</v>
       </c>
       <c r="B3" s="8">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="C3" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1427,10 +1438,10 @@
         <v>120</v>
       </c>
       <c r="B4" s="8">
-        <v>135</v>
+        <v>142</v>
       </c>
       <c r="C4" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1438,10 +1449,10 @@
         <v>121</v>
       </c>
       <c r="B5" s="8">
-        <v>429</v>
+        <v>482</v>
       </c>
       <c r="C5" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1449,10 +1460,10 @@
         <v>122</v>
       </c>
       <c r="B6" s="8">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C6" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1463,7 +1474,7 @@
         <v>52</v>
       </c>
       <c r="C7" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1474,7 +1485,7 @@
         <v>43</v>
       </c>
       <c r="C8" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1482,10 +1493,10 @@
         <v>125</v>
       </c>
       <c r="B9" s="8">
-        <v>150</v>
+        <v>164</v>
       </c>
       <c r="C9" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -1493,10 +1504,10 @@
         <v>126</v>
       </c>
       <c r="B10" s="8">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="C10" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -1504,10 +1515,10 @@
         <v>127</v>
       </c>
       <c r="B11" s="8">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C11" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1515,10 +1526,10 @@
         <v>128</v>
       </c>
       <c r="B12" s="8">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="C12" s="9">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -1526,10 +1537,10 @@
         <v>118</v>
       </c>
       <c r="B13" s="8">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="C13" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -1537,10 +1548,10 @@
         <v>119</v>
       </c>
       <c r="B14" s="8">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="C14" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1548,10 +1559,10 @@
         <v>120</v>
       </c>
       <c r="B15" s="8">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="C15" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -1559,10 +1570,10 @@
         <v>121</v>
       </c>
       <c r="B16" s="8">
-        <v>396</v>
+        <v>429</v>
       </c>
       <c r="C16" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -1570,10 +1581,10 @@
         <v>122</v>
       </c>
       <c r="B17" s="8">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="C17" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -1584,7 +1595,7 @@
         <v>52</v>
       </c>
       <c r="C18" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -1595,7 +1606,7 @@
         <v>43</v>
       </c>
       <c r="C19" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
@@ -1603,10 +1614,10 @@
         <v>125</v>
       </c>
       <c r="B20" s="8">
-        <v>143</v>
+        <v>150</v>
       </c>
       <c r="C20" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
@@ -1614,10 +1625,10 @@
         <v>126</v>
       </c>
       <c r="B21" s="8">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C21" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
@@ -1625,10 +1636,10 @@
         <v>127</v>
       </c>
       <c r="B22" s="8">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="C22" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
@@ -1636,10 +1647,10 @@
         <v>128</v>
       </c>
       <c r="B23" s="8">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="C23" s="9">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
@@ -1647,10 +1658,10 @@
         <v>118</v>
       </c>
       <c r="B24" s="8">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C24" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
@@ -1658,10 +1669,10 @@
         <v>119</v>
       </c>
       <c r="B25" s="8">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="C25" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
@@ -1669,10 +1680,10 @@
         <v>120</v>
       </c>
       <c r="B26" s="8">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="C26" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
@@ -1680,10 +1691,10 @@
         <v>121</v>
       </c>
       <c r="B27" s="8">
-        <v>377</v>
+        <v>396</v>
       </c>
       <c r="C27" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1691,10 +1702,10 @@
         <v>122</v>
       </c>
       <c r="B28" s="8">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="C28" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
@@ -1702,10 +1713,10 @@
         <v>123</v>
       </c>
       <c r="B29" s="8">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C29" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
@@ -1713,10 +1724,10 @@
         <v>124</v>
       </c>
       <c r="B30" s="8">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C30" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
@@ -1724,10 +1735,10 @@
         <v>125</v>
       </c>
       <c r="B31" s="8">
-        <v>130</v>
+        <v>143</v>
       </c>
       <c r="C31" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
@@ -1735,10 +1746,10 @@
         <v>126</v>
       </c>
       <c r="B32" s="8">
-        <v>59</v>
+        <v>69</v>
       </c>
       <c r="C32" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
@@ -1746,10 +1757,10 @@
         <v>127</v>
       </c>
       <c r="B33" s="8">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="C33" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
@@ -1757,10 +1768,10 @@
         <v>128</v>
       </c>
       <c r="B34" s="8">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="C34" s="9">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
@@ -1768,10 +1779,10 @@
         <v>118</v>
       </c>
       <c r="B35" s="8">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C35" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
@@ -1779,10 +1790,10 @@
         <v>119</v>
       </c>
       <c r="B36" s="8">
-        <v>81</v>
+        <v>102</v>
       </c>
       <c r="C36" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
@@ -1790,10 +1801,10 @@
         <v>120</v>
       </c>
       <c r="B37" s="8">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="C37" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
@@ -1801,10 +1812,10 @@
         <v>121</v>
       </c>
       <c r="B38" s="8">
-        <v>272</v>
+        <v>377</v>
       </c>
       <c r="C38" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
@@ -1812,10 +1823,10 @@
         <v>122</v>
       </c>
       <c r="B39" s="8">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C39" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
@@ -1823,10 +1834,10 @@
         <v>123</v>
       </c>
       <c r="B40" s="8">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C40" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
@@ -1834,10 +1845,10 @@
         <v>124</v>
       </c>
       <c r="B41" s="8">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C41" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
@@ -1845,10 +1856,10 @@
         <v>125</v>
       </c>
       <c r="B42" s="8">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="C42" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
@@ -1856,10 +1867,10 @@
         <v>126</v>
       </c>
       <c r="B43" s="8">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="C43" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
@@ -1867,10 +1878,10 @@
         <v>127</v>
       </c>
       <c r="B44" s="8">
-        <v>23</v>
+        <v>33</v>
       </c>
       <c r="C44" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
@@ -1878,10 +1889,10 @@
         <v>128</v>
       </c>
       <c r="B45" s="8">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="C45" s="9">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
@@ -1889,120 +1900,120 @@
         <v>118</v>
       </c>
       <c r="B46" s="8">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="C46" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B47" s="8">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C47" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48" s="8" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B48" s="8">
-        <v>226</v>
+        <v>91</v>
       </c>
       <c r="C48" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" s="8" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B49" s="8">
-        <v>19</v>
+        <v>272</v>
       </c>
       <c r="C49" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50" s="8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B50" s="8">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="C50" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51" s="8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B51" s="8">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C51" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52" s="8" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B52" s="8">
-        <v>97</v>
+        <v>40</v>
       </c>
       <c r="C52" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B53" s="8">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="C53" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54" s="8" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B54" s="8">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C54" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55" s="8" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B55" s="8">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="C55" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56" s="8" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B56" s="8">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="C56" s="9">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
@@ -2010,10 +2021,10 @@
         <v>118</v>
       </c>
       <c r="B57" s="8">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C57" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
@@ -2021,10 +2032,10 @@
         <v>120</v>
       </c>
       <c r="B58" s="8">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C58" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
@@ -2032,10 +2043,10 @@
         <v>121</v>
       </c>
       <c r="B59" s="8">
-        <v>200</v>
+        <v>226</v>
       </c>
       <c r="C59" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
@@ -2043,10 +2054,10 @@
         <v>122</v>
       </c>
       <c r="B60" s="8">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C60" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
@@ -2054,10 +2065,10 @@
         <v>123</v>
       </c>
       <c r="B61" s="8">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C61" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
@@ -2065,10 +2076,10 @@
         <v>124</v>
       </c>
       <c r="B62" s="8">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="C62" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
@@ -2076,10 +2087,10 @@
         <v>125</v>
       </c>
       <c r="B63" s="8">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="C63" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
@@ -2087,10 +2098,10 @@
         <v>126</v>
       </c>
       <c r="B64" s="8">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C64" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -2098,10 +2109,10 @@
         <v>127</v>
       </c>
       <c r="B65" s="8">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C65" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
@@ -2109,10 +2120,10 @@
         <v>128</v>
       </c>
       <c r="B66" s="8">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C66" s="9">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -2120,9 +2131,130 @@
         <v>129</v>
       </c>
       <c r="B67" s="8">
+        <v>75</v>
+      </c>
+      <c r="C67" s="9">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="B68" s="8">
+        <v>47</v>
+      </c>
+      <c r="C68" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B69" s="8">
+        <v>70</v>
+      </c>
+      <c r="C69" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="B70" s="8">
+        <v>200</v>
+      </c>
+      <c r="C70" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="B71" s="8">
+        <v>18</v>
+      </c>
+      <c r="C71" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B72" s="8">
+        <v>29</v>
+      </c>
+      <c r="C72" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="B73" s="8">
+        <v>32</v>
+      </c>
+      <c r="C73" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="B74" s="8">
+        <v>81</v>
+      </c>
+      <c r="C74" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="B75" s="8">
+        <v>36</v>
+      </c>
+      <c r="C75" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="B76" s="8">
+        <v>19</v>
+      </c>
+      <c r="C76" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B77" s="8">
+        <v>51</v>
+      </c>
+      <c r="C77" s="9">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="B78" s="8">
         <v>67</v>
       </c>
-      <c r="C67" s="9">
+      <c r="C78" s="9">
         <v>43922</v>
       </c>
     </row>
@@ -2255,13 +2387,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K31"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomRight" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3295,35 +3427,35 @@
         <v>43928</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C30" s="5">
-        <v>5709</v>
+        <v>6444</v>
       </c>
       <c r="D30" s="5">
         <f>C30-C29</f>
-        <v>-272</v>
-      </c>
-      <c r="E30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="5" t="s">
-        <v>8</v>
+        <v>463</v>
+      </c>
+      <c r="E30" s="5">
+        <v>1521</v>
+      </c>
+      <c r="F30" s="5">
+        <v>230</v>
       </c>
       <c r="G30" s="5">
-        <v>210</v>
-      </c>
-      <c r="H30" t="s">
-        <v>8</v>
-      </c>
-      <c r="I30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J30" s="5" t="s">
-        <v>8</v>
+        <v>257</v>
+      </c>
+      <c r="H30">
+        <v>1765</v>
+      </c>
+      <c r="I30" s="5">
+        <v>317</v>
+      </c>
+      <c r="J30" s="5">
+        <v>48</v>
       </c>
       <c r="K30" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -3338,7 +3470,7 @@
       </c>
       <c r="D31" s="5">
         <f>C31-C30</f>
-        <v>365</v>
+        <v>-370</v>
       </c>
       <c r="E31" t="s">
         <v>8</v>
@@ -3360,6 +3492,42 @@
       </c>
       <c r="K31" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B32" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C32">
+        <f>C31+D32</f>
+        <v>6574</v>
+      </c>
+      <c r="D32">
+        <v>500</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" t="s">
+        <v>8</v>
+      </c>
+      <c r="G32" s="5">
+        <v>263</v>
+      </c>
+      <c r="H32" t="s">
+        <v>8</v>
+      </c>
+      <c r="I32" t="s">
+        <v>8</v>
+      </c>
+      <c r="J32" t="s">
+        <v>8</v>
+      </c>
+      <c r="K32" t="s">
+        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -3369,10 +3537,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B646AB9-6DFD-6342-9B5D-CA852E35631D}">
-  <dimension ref="A1:D62"/>
+  <dimension ref="A1:D65"/>
   <sheetViews>
     <sheetView topLeftCell="A34" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A60" sqref="A60:A62"/>
+      <selection activeCell="A63" sqref="A63:A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4248,6 +4416,48 @@
         <v>1.2</v>
       </c>
     </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B63" t="s">
+        <v>61</v>
+      </c>
+      <c r="C63">
+        <v>3425</v>
+      </c>
+      <c r="D63">
+        <v>53.2</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B64" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64">
+        <v>2923</v>
+      </c>
+      <c r="D64">
+        <v>45.4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A65" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B65" t="s">
+        <v>52</v>
+      </c>
+      <c r="C65">
+        <v>96</v>
+      </c>
+      <c r="D65">
+        <v>1.5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4255,11 +4465,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2CC04-F5BC-6741-A3F2-2661873C87D7}">
-  <dimension ref="A1:E237"/>
+  <dimension ref="A1:E248"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D231" sqref="D231"/>
+      <selection pane="bottomLeft" activeCell="C240" sqref="C240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -7465,12 +7675,6 @@
       <c r="A229" s="1">
         <v>43927</v>
       </c>
-      <c r="B229" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="C229" t="s">
-        <v>8</v>
-      </c>
       <c r="D229">
         <v>7</v>
       </c>
@@ -7584,6 +7788,161 @@
         <v>17</v>
       </c>
       <c r="D237">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A238" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B238" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C238">
+        <v>14</v>
+      </c>
+      <c r="D238" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A239" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B239" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C239">
+        <v>19</v>
+      </c>
+      <c r="D239" t="s">
+        <v>8</v>
+      </c>
+      <c r="E239" s="7"/>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A240" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B240" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C240" t="s">
+        <v>8</v>
+      </c>
+      <c r="D240">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="241" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A241" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B241" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C241">
+        <v>43</v>
+      </c>
+      <c r="D241">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="242" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A242" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B242" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C242">
+        <v>384</v>
+      </c>
+      <c r="D242">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="243" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A243" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B243" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C243">
+        <v>1103</v>
+      </c>
+      <c r="D243">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="244" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A244" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B244" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C244">
+        <v>1176</v>
+      </c>
+      <c r="D244">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="245" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A245" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B245" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C245">
+        <v>1219</v>
+      </c>
+      <c r="D245">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="246" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A246" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B246" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C246">
+        <v>922</v>
+      </c>
+      <c r="D246">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="247" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B247" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C247">
+        <v>1544</v>
+      </c>
+      <c r="D247">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="248" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B248" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C248">
+        <v>20</v>
+      </c>
+      <c r="D248">
         <v>2</v>
       </c>
     </row>
@@ -7594,17 +7953,18 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029AF1D0-4AE1-A540-B628-AF7C84CE0F40}">
-  <dimension ref="A1:D82"/>
+  <dimension ref="A1:D85"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79:D82"/>
+      <selection pane="bottomLeft" activeCell="A83" sqref="A83:A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -7614,7 +7974,7 @@
       <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="11" t="s">
         <v>55</v>
       </c>
       <c r="D1" t="s">
@@ -7628,7 +7988,7 @@
       <c r="B2" t="s">
         <v>56</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="11">
         <v>2</v>
       </c>
       <c r="D2" t="s">
@@ -7642,7 +8002,7 @@
       <c r="B3" t="s">
         <v>57</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="11">
         <v>22</v>
       </c>
       <c r="D3" t="s">
@@ -7656,7 +8016,7 @@
       <c r="B4" t="s">
         <v>58</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="11">
         <v>3</v>
       </c>
       <c r="D4" t="s">
@@ -7670,7 +8030,7 @@
       <c r="B5" t="s">
         <v>56</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="11">
         <v>2</v>
       </c>
       <c r="D5" t="s">
@@ -7684,7 +8044,7 @@
       <c r="B6" t="s">
         <v>57</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="11">
         <v>12</v>
       </c>
       <c r="D6" t="s">
@@ -7698,7 +8058,7 @@
       <c r="B7" t="s">
         <v>58</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="11">
         <v>6</v>
       </c>
       <c r="D7" t="s">
@@ -7712,7 +8072,7 @@
       <c r="B8" t="s">
         <v>56</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="11">
         <v>60</v>
       </c>
       <c r="D8" t="s">
@@ -7726,7 +8086,7 @@
       <c r="B9" t="s">
         <v>57</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="11">
         <v>45</v>
       </c>
       <c r="D9" t="s">
@@ -7740,7 +8100,7 @@
       <c r="B10" t="s">
         <v>58</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="11">
         <v>113</v>
       </c>
       <c r="D10" t="s">
@@ -7754,7 +8114,7 @@
       <c r="B11" t="s">
         <v>59</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="11">
         <v>53</v>
       </c>
       <c r="D11" t="s">
@@ -7768,7 +8128,7 @@
       <c r="B12" t="s">
         <v>56</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="11">
         <v>99</v>
       </c>
       <c r="D12" t="s">
@@ -7782,7 +8142,7 @@
       <c r="B13" t="s">
         <v>57</v>
       </c>
-      <c r="C13">
+      <c r="C13" s="11">
         <v>59</v>
       </c>
       <c r="D13" t="s">
@@ -7796,7 +8156,7 @@
       <c r="B14" t="s">
         <v>58</v>
       </c>
-      <c r="C14">
+      <c r="C14" s="11">
         <v>121</v>
       </c>
       <c r="D14" t="s">
@@ -7810,7 +8170,7 @@
       <c r="B15" t="s">
         <v>59</v>
       </c>
-      <c r="C15">
+      <c r="C15" s="11">
         <v>71</v>
       </c>
       <c r="D15" t="s">
@@ -7824,7 +8184,7 @@
       <c r="B16" t="s">
         <v>56</v>
       </c>
-      <c r="C16">
+      <c r="C16" s="11">
         <v>40</v>
       </c>
       <c r="D16" t="s">
@@ -7838,7 +8198,7 @@
       <c r="B17" t="s">
         <v>57</v>
       </c>
-      <c r="C17">
+      <c r="C17" s="11">
         <v>21</v>
       </c>
       <c r="D17" t="s">
@@ -7852,7 +8212,7 @@
       <c r="B18" t="s">
         <v>58</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="11">
         <v>39</v>
       </c>
       <c r="D18" t="s">
@@ -7866,7 +8226,7 @@
       <c r="B19" t="s">
         <v>59</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="11">
         <v>96</v>
       </c>
       <c r="D19" t="s">
@@ -7880,7 +8240,7 @@
       <c r="B20" t="s">
         <v>56</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="11">
         <v>179</v>
       </c>
       <c r="D20" t="s">
@@ -7894,7 +8254,7 @@
       <c r="B21" t="s">
         <v>57</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="11">
         <v>97</v>
       </c>
       <c r="D21" t="s">
@@ -7908,7 +8268,7 @@
       <c r="B22" t="s">
         <v>58</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="11">
         <v>148</v>
       </c>
       <c r="D22" t="s">
@@ -7922,7 +8282,7 @@
       <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="11">
         <v>160</v>
       </c>
       <c r="D23" t="s">
@@ -7936,7 +8296,7 @@
       <c r="B24" t="s">
         <v>56</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="11">
         <v>44</v>
       </c>
       <c r="D24" t="s">
@@ -7950,7 +8310,7 @@
       <c r="B25" t="s">
         <v>57</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="11">
         <v>23</v>
       </c>
       <c r="D25" t="s">
@@ -7964,7 +8324,7 @@
       <c r="B26" t="s">
         <v>58</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="11">
         <v>33</v>
       </c>
       <c r="D26" t="s">
@@ -7978,7 +8338,7 @@
       <c r="B27" t="s">
         <v>59</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="11">
         <v>258</v>
       </c>
       <c r="D27" t="s">
@@ -7992,7 +8352,7 @@
       <c r="B28" t="s">
         <v>56</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="11">
         <v>43</v>
       </c>
       <c r="D28" t="s">
@@ -8006,7 +8366,7 @@
       <c r="B29" t="s">
         <v>57</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="11">
         <v>24</v>
       </c>
       <c r="D29" t="s">
@@ -8020,7 +8380,7 @@
       <c r="B30" t="s">
         <v>58</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="11">
         <v>33</v>
       </c>
       <c r="D30" t="s">
@@ -8034,7 +8394,7 @@
       <c r="B31" t="s">
         <v>56</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="11">
         <v>45</v>
       </c>
       <c r="D31" t="s">
@@ -8048,7 +8408,7 @@
       <c r="B32" t="s">
         <v>57</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="11">
         <v>24</v>
       </c>
       <c r="D32" t="s">
@@ -8062,7 +8422,7 @@
       <c r="B33" t="s">
         <v>58</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="11">
         <v>31</v>
       </c>
       <c r="D33" t="s">
@@ -8076,7 +8436,7 @@
       <c r="B34" t="s">
         <v>56</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="11">
         <v>29</v>
       </c>
       <c r="D34" t="s">
@@ -8090,7 +8450,7 @@
       <c r="B35" t="s">
         <v>57</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="11">
         <v>15</v>
       </c>
       <c r="D35" t="s">
@@ -8104,7 +8464,7 @@
       <c r="B36" t="s">
         <v>58</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="11">
         <v>18</v>
       </c>
       <c r="D36" t="s">
@@ -8118,7 +8478,7 @@
       <c r="B37" t="s">
         <v>59</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="11">
         <v>38</v>
       </c>
       <c r="D37" t="s">
@@ -8132,7 +8492,7 @@
       <c r="B38" t="s">
         <v>56</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="11">
         <v>28</v>
       </c>
       <c r="D38" t="s">
@@ -8146,7 +8506,7 @@
       <c r="B39" t="s">
         <v>57</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="11">
         <v>13</v>
       </c>
       <c r="D39" t="s">
@@ -8160,7 +8520,7 @@
       <c r="B40" t="s">
         <v>58</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="11">
         <v>16</v>
       </c>
       <c r="D40" t="s">
@@ -8174,7 +8534,7 @@
       <c r="B41" t="s">
         <v>59</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="11">
         <v>42</v>
       </c>
       <c r="D41" t="s">
@@ -8188,7 +8548,7 @@
       <c r="B42" t="s">
         <v>56</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="11">
         <v>28</v>
       </c>
       <c r="D42" t="s">
@@ -8202,7 +8562,7 @@
       <c r="B43" t="s">
         <v>57</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="11">
         <v>12</v>
       </c>
       <c r="D43" t="s">
@@ -8216,7 +8576,7 @@
       <c r="B44" t="s">
         <v>58</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="11">
         <v>15</v>
       </c>
       <c r="D44" t="s">
@@ -8230,7 +8590,7 @@
       <c r="B45" t="s">
         <v>59</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="11">
         <v>45</v>
       </c>
       <c r="D45" t="s">
@@ -8244,7 +8604,7 @@
       <c r="B46" t="s">
         <v>56</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="11">
         <v>25</v>
       </c>
       <c r="D46" t="s">
@@ -8258,7 +8618,7 @@
       <c r="B47" t="s">
         <v>57</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="11">
         <v>12</v>
       </c>
       <c r="D47" t="s">
@@ -8272,7 +8632,7 @@
       <c r="B48" t="s">
         <v>58</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="11">
         <v>13</v>
       </c>
       <c r="D48" t="s">
@@ -8286,7 +8646,7 @@
       <c r="B49" t="s">
         <v>59</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="11">
         <v>55</v>
       </c>
       <c r="D49" t="s">
@@ -8300,7 +8660,7 @@
       <c r="B50" t="s">
         <v>56</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="11">
         <v>51</v>
       </c>
       <c r="D50" t="s">
@@ -8314,7 +8674,7 @@
       <c r="B51" t="s">
         <v>57</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="11">
         <v>25</v>
       </c>
       <c r="D51" t="s">
@@ -8328,7 +8688,7 @@
       <c r="B52" t="s">
         <v>58</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="11">
         <v>24</v>
       </c>
       <c r="D52" t="s">
@@ -8342,7 +8702,7 @@
       <c r="B53" t="s">
         <v>56</v>
       </c>
-      <c r="C53">
+      <c r="C53" s="11">
         <v>50</v>
       </c>
       <c r="D53" t="s">
@@ -8356,7 +8716,7 @@
       <c r="B54" t="s">
         <v>57</v>
       </c>
-      <c r="C54">
+      <c r="C54" s="11">
         <v>27</v>
       </c>
       <c r="D54" t="s">
@@ -8370,7 +8730,7 @@
       <c r="B55" t="s">
         <v>58</v>
       </c>
-      <c r="C55">
+      <c r="C55" s="11">
         <v>23</v>
       </c>
       <c r="D55" t="s">
@@ -8384,7 +8744,7 @@
       <c r="B56" t="s">
         <v>56</v>
       </c>
-      <c r="C56">
+      <c r="C56" s="11">
         <v>51</v>
       </c>
       <c r="D56" t="s">
@@ -8398,7 +8758,7 @@
       <c r="B57" t="s">
         <v>57</v>
       </c>
-      <c r="C57">
+      <c r="C57" s="11">
         <v>26</v>
       </c>
       <c r="D57" t="s">
@@ -8412,7 +8772,7 @@
       <c r="B58" t="s">
         <v>58</v>
       </c>
-      <c r="C58">
+      <c r="C58" s="11">
         <v>23</v>
       </c>
       <c r="D58" t="s">
@@ -8426,7 +8786,7 @@
       <c r="B59" t="s">
         <v>56</v>
       </c>
-      <c r="C59">
+      <c r="C59" s="11">
         <v>60</v>
       </c>
       <c r="D59" t="s">
@@ -8440,7 +8800,7 @@
       <c r="B60" t="s">
         <v>57</v>
       </c>
-      <c r="C60">
+      <c r="C60" s="11">
         <v>21</v>
       </c>
       <c r="D60" t="s">
@@ -8454,7 +8814,7 @@
       <c r="B61" t="s">
         <v>58</v>
       </c>
-      <c r="C61">
+      <c r="C61" s="11">
         <v>19</v>
       </c>
       <c r="D61" t="s">
@@ -8468,7 +8828,7 @@
       <c r="B62" t="s">
         <v>56</v>
       </c>
-      <c r="C62">
+      <c r="C62" s="11">
         <v>59</v>
       </c>
       <c r="D62" t="s">
@@ -8482,7 +8842,7 @@
       <c r="B63" t="s">
         <v>57</v>
       </c>
-      <c r="C63">
+      <c r="C63" s="11">
         <v>23</v>
       </c>
       <c r="D63" t="s">
@@ -8496,7 +8856,7 @@
       <c r="B64" t="s">
         <v>58</v>
       </c>
-      <c r="C64">
+      <c r="C64" s="11">
         <v>18</v>
       </c>
       <c r="D64" t="s">
@@ -8510,7 +8870,7 @@
       <c r="B65" t="s">
         <v>56</v>
       </c>
-      <c r="C65">
+      <c r="C65" s="11">
         <v>61</v>
       </c>
       <c r="D65" t="s">
@@ -8524,7 +8884,7 @@
       <c r="B66" t="s">
         <v>57</v>
       </c>
-      <c r="C66">
+      <c r="C66" s="11">
         <v>23</v>
       </c>
       <c r="D66" t="s">
@@ -8538,7 +8898,7 @@
       <c r="B67" t="s">
         <v>58</v>
       </c>
-      <c r="C67">
+      <c r="C67" s="11">
         <v>16</v>
       </c>
       <c r="D67" t="s">
@@ -8552,7 +8912,7 @@
       <c r="B68" t="s">
         <v>56</v>
       </c>
-      <c r="C68">
+      <c r="C68" s="11">
         <v>62</v>
       </c>
       <c r="D68" t="s">
@@ -8566,7 +8926,7 @@
       <c r="B69" t="s">
         <v>57</v>
       </c>
-      <c r="C69">
+      <c r="C69" s="11">
         <v>23</v>
       </c>
       <c r="D69" t="s">
@@ -8580,7 +8940,7 @@
       <c r="B70" t="s">
         <v>58</v>
       </c>
-      <c r="C70">
+      <c r="C70" s="11">
         <v>15</v>
       </c>
       <c r="D70" t="s">
@@ -8594,7 +8954,7 @@
       <c r="B71" t="s">
         <v>56</v>
       </c>
-      <c r="C71">
+      <c r="C71" s="11">
         <v>63</v>
       </c>
       <c r="D71" t="s">
@@ -8608,7 +8968,7 @@
       <c r="B72" t="s">
         <v>57</v>
       </c>
-      <c r="C72">
+      <c r="C72" s="11">
         <v>24</v>
       </c>
       <c r="D72" t="s">
@@ -8622,7 +8982,7 @@
       <c r="B73" t="s">
         <v>58</v>
       </c>
-      <c r="C73">
+      <c r="C73" s="11">
         <v>13</v>
       </c>
       <c r="D73" t="s">
@@ -8636,7 +8996,7 @@
       <c r="B74" t="s">
         <v>56</v>
       </c>
-      <c r="C74">
+      <c r="C74" s="11">
         <v>65</v>
       </c>
       <c r="D74" t="s">
@@ -8650,7 +9010,7 @@
       <c r="B75" t="s">
         <v>57</v>
       </c>
-      <c r="C75">
+      <c r="C75" s="11">
         <v>23</v>
       </c>
       <c r="D75" t="s">
@@ -8664,7 +9024,7 @@
       <c r="B76" t="s">
         <v>58</v>
       </c>
-      <c r="C76">
+      <c r="C76" s="11">
         <v>12</v>
       </c>
       <c r="D76" t="s">
@@ -8678,7 +9038,7 @@
       <c r="B77" t="s">
         <v>56</v>
       </c>
-      <c r="C77">
+      <c r="C77" s="11">
         <v>67</v>
       </c>
       <c r="D77" t="s">
@@ -8692,7 +9052,7 @@
       <c r="B78" t="s">
         <v>57</v>
       </c>
-      <c r="C78">
+      <c r="C78" s="11">
         <v>22</v>
       </c>
       <c r="D78" t="s">
@@ -8706,7 +9066,7 @@
       <c r="B79" t="s">
         <v>58</v>
       </c>
-      <c r="C79">
+      <c r="C79" s="11">
         <v>11</v>
       </c>
       <c r="D79" t="s">
@@ -8720,7 +9080,7 @@
       <c r="B80" t="s">
         <v>56</v>
       </c>
-      <c r="C80">
+      <c r="C80" s="11">
         <v>67</v>
       </c>
       <c r="D80" t="s">
@@ -8734,7 +9094,7 @@
       <c r="B81" t="s">
         <v>57</v>
       </c>
-      <c r="C81">
+      <c r="C81" s="11">
         <v>23</v>
       </c>
       <c r="D81" t="s">
@@ -8748,10 +9108,52 @@
       <c r="B82" t="s">
         <v>58</v>
       </c>
-      <c r="C82">
+      <c r="C82" s="11">
         <v>10</v>
       </c>
       <c r="D82" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+      <c r="C83" s="11">
+        <v>67</v>
+      </c>
+      <c r="D83" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B84" t="s">
+        <v>57</v>
+      </c>
+      <c r="C84" s="11">
+        <v>24</v>
+      </c>
+      <c r="D84" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B85" t="s">
+        <v>58</v>
+      </c>
+      <c r="C85" s="11">
+        <v>9</v>
+      </c>
+      <c r="D85" t="s">
         <v>106</v>
       </c>
     </row>
@@ -8762,10 +9164,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77735C93-7ED9-C044-B61C-E23C86F44D03}">
-  <dimension ref="A1:E567"/>
+  <dimension ref="A1:E593"/>
   <sheetViews>
-    <sheetView topLeftCell="A533" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A542" sqref="A542:A567"/>
+    <sheetView topLeftCell="A557" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A568" sqref="A568:A593"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17200,6 +17602,370 @@
         <v>0.03</v>
       </c>
     </row>
+    <row r="568" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A568" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B568" t="s">
+        <v>12</v>
+      </c>
+      <c r="C568">
+        <v>16</v>
+      </c>
+      <c r="D568" s="3">
+        <v>2E-3</v>
+      </c>
+    </row>
+    <row r="569" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A569" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B569" t="s">
+        <v>14</v>
+      </c>
+      <c r="C569">
+        <v>132</v>
+      </c>
+      <c r="D569" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="570" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A570" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B570" t="s">
+        <v>15</v>
+      </c>
+      <c r="C570">
+        <v>68</v>
+      </c>
+      <c r="D570" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="571" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A571" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B571" t="s">
+        <v>16</v>
+      </c>
+      <c r="C571">
+        <v>472</v>
+      </c>
+      <c r="D571" s="3">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="572" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A572" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B572" t="s">
+        <v>17</v>
+      </c>
+      <c r="C572">
+        <v>125</v>
+      </c>
+      <c r="D572" s="3">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="573" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A573" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B573" t="s">
+        <v>18</v>
+      </c>
+      <c r="C573">
+        <v>3557</v>
+      </c>
+      <c r="D573" s="3">
+        <v>0.55200000000000005</v>
+      </c>
+    </row>
+    <row r="574" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A574" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B574" t="s">
+        <v>19</v>
+      </c>
+      <c r="C574">
+        <v>134</v>
+      </c>
+      <c r="D574" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="575" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A575" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B575" t="s">
+        <v>20</v>
+      </c>
+      <c r="C575">
+        <v>125</v>
+      </c>
+      <c r="D575" s="3">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="576" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A576" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B576" t="s">
+        <v>21</v>
+      </c>
+      <c r="C576">
+        <v>253</v>
+      </c>
+      <c r="D576" s="3">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="577" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A577" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B577" t="s">
+        <v>22</v>
+      </c>
+      <c r="C577">
+        <v>90</v>
+      </c>
+      <c r="D577" s="3">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="578" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A578" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B578" t="s">
+        <v>36</v>
+      </c>
+      <c r="C578">
+        <v>37</v>
+      </c>
+      <c r="D578" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="579" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A579" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B579" t="s">
+        <v>37</v>
+      </c>
+      <c r="C579">
+        <v>23</v>
+      </c>
+      <c r="D579" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="580" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A580" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B580" t="s">
+        <v>23</v>
+      </c>
+      <c r="C580">
+        <v>173</v>
+      </c>
+      <c r="D580" s="3">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="581" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A581" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B581" t="s">
+        <v>24</v>
+      </c>
+      <c r="C581">
+        <v>36</v>
+      </c>
+      <c r="D581" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="582" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A582" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B582" t="s">
+        <v>25</v>
+      </c>
+      <c r="C582">
+        <v>106</v>
+      </c>
+      <c r="D582" s="3">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="583" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A583" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B583" t="s">
+        <v>26</v>
+      </c>
+      <c r="C583">
+        <v>134</v>
+      </c>
+      <c r="D583" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="584" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A584" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B584" t="s">
+        <v>27</v>
+      </c>
+      <c r="C584">
+        <v>198</v>
+      </c>
+      <c r="D584" s="3">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="585" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A585" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B585" t="s">
+        <v>38</v>
+      </c>
+      <c r="C585">
+        <v>63</v>
+      </c>
+      <c r="D585" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="586" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A586" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B586" t="s">
+        <v>28</v>
+      </c>
+      <c r="C586">
+        <v>81</v>
+      </c>
+      <c r="D586" s="3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="587" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A587" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B587" t="s">
+        <v>29</v>
+      </c>
+      <c r="C587">
+        <v>22</v>
+      </c>
+      <c r="D587" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="588" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A588" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B588" t="s">
+        <v>30</v>
+      </c>
+      <c r="C588">
+        <v>28</v>
+      </c>
+      <c r="D588" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="589" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A589" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B589" t="s">
+        <v>31</v>
+      </c>
+      <c r="C589">
+        <v>140</v>
+      </c>
+      <c r="D589" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="590" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A590" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B590" t="s">
+        <v>32</v>
+      </c>
+      <c r="C590">
+        <v>56</v>
+      </c>
+      <c r="D590" s="3">
+        <v>8.9999999999999993E-3</v>
+      </c>
+    </row>
+    <row r="591" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A591" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B591" t="s">
+        <v>33</v>
+      </c>
+      <c r="C591">
+        <v>142</v>
+      </c>
+      <c r="D591" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="592" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A592" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B592" t="s">
+        <v>34</v>
+      </c>
+      <c r="C592">
+        <v>26</v>
+      </c>
+      <c r="D592" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A593" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B593" t="s">
+        <v>35</v>
+      </c>
+      <c r="C593">
+        <v>207</v>
+      </c>
+      <c r="D593" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17207,9 +17973,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE73A96-9009-C14A-A4D6-627BDCEBA7A8}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -17243,192 +18009,216 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43929</v>
+        <v>43930</v>
       </c>
       <c r="B2">
-        <v>84</v>
+        <v>138</v>
       </c>
       <c r="C2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D2">
-        <v>1339</v>
+        <v>1477</v>
       </c>
       <c r="E2">
-        <v>78</v>
+        <v>82</v>
       </c>
       <c r="F2">
-        <v>9564</v>
+        <v>10203</v>
       </c>
       <c r="G2" s="10">
         <f>D2/F2</f>
-        <v>0.14000418235048098</v>
+        <v>0.14476134470253846</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43928</v>
+        <v>43929</v>
       </c>
       <c r="B3">
-        <v>97</v>
+        <v>84</v>
       </c>
       <c r="C3">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>1255</v>
+        <v>1339</v>
       </c>
       <c r="E3">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F3">
-        <v>9158</v>
+        <v>9564</v>
       </c>
       <c r="G3" s="10">
-        <f t="shared" ref="G3:G9" si="0">D3/F3</f>
-        <v>0.13703865472810658</v>
+        <f>D3/F3</f>
+        <v>0.14000418235048098</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B4">
+        <v>97</v>
+      </c>
+      <c r="C4">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>1255</v>
+      </c>
+      <c r="E4">
+        <v>73</v>
+      </c>
+      <c r="F4">
+        <v>9158</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" ref="G4:G10" si="0">D4/F4</f>
+        <v>0.13703865472810658</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
         <v>43927</v>
       </c>
-      <c r="B4">
+      <c r="B5">
         <v>69</v>
       </c>
-      <c r="C4">
+      <c r="C5">
         <v>7</v>
       </c>
-      <c r="D4">
+      <c r="D5">
         <v>1158</v>
       </c>
-      <c r="E4">
+      <c r="E5">
         <v>70</v>
       </c>
-      <c r="F4">
+      <c r="F5">
         <v>8740</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G5" s="10">
         <f t="shared" si="0"/>
         <v>0.13249427917620138</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
         <v>43926</v>
       </c>
-      <c r="B5">
+      <c r="B6">
         <v>91</v>
       </c>
-      <c r="C5">
+      <c r="C6">
         <v>7</v>
       </c>
-      <c r="D5">
+      <c r="D6">
         <v>1089</v>
       </c>
-      <c r="E5">
+      <c r="E6">
         <v>63</v>
       </c>
-      <c r="F5">
+      <c r="F6">
         <v>8486</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G6" s="10">
         <f t="shared" si="0"/>
         <v>0.12832901249116191</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
         <v>43925</v>
       </c>
-      <c r="B6">
+      <c r="B7">
         <v>94</v>
       </c>
-      <c r="C6">
-        <v>8</v>
-      </c>
-      <c r="D6">
+      <c r="C7">
+        <v>8</v>
+      </c>
+      <c r="D7">
         <v>998</v>
       </c>
-      <c r="E6">
+      <c r="E7">
         <v>56</v>
       </c>
-      <c r="F6">
+      <c r="F7">
         <v>8034</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G7" s="10">
         <f t="shared" si="0"/>
         <v>0.12422205626089121</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="1">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
         <v>43924</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>130</v>
       </c>
-      <c r="C7">
+      <c r="C8">
         <v>12</v>
       </c>
-      <c r="D7">
+      <c r="D8">
         <v>904</v>
       </c>
-      <c r="E7">
+      <c r="E8">
         <v>48</v>
       </c>
-      <c r="F7">
+      <c r="F8">
         <v>7525</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G8" s="10">
         <f t="shared" si="0"/>
         <v>0.12013289036544851</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="1">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
         <v>43923</v>
       </c>
-      <c r="B8">
+      <c r="B9">
         <v>85</v>
       </c>
-      <c r="C8">
+      <c r="C9">
         <v>6</v>
       </c>
-      <c r="D8">
+      <c r="D9">
         <v>774</v>
       </c>
-      <c r="E8">
+      <c r="E9">
         <v>36</v>
       </c>
-      <c r="F8">
+      <c r="F9">
         <v>6899</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G9" s="10">
         <f t="shared" si="0"/>
         <v>0.11219017248876649</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
         <v>43922</v>
       </c>
-      <c r="B9">
+      <c r="B10">
         <v>103</v>
       </c>
-      <c r="C9">
+      <c r="C10">
         <v>2</v>
       </c>
-      <c r="D9">
+      <c r="D10">
         <v>689</v>
       </c>
-      <c r="E9">
+      <c r="E10">
         <v>30</v>
       </c>
-      <c r="F9">
+      <c r="F10">
         <v>6450</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G10" s="10">
         <f t="shared" si="0"/>
         <v>0.10682170542635659</v>
       </c>
@@ -17440,10 +18230,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0979910-C687-6A43-A609-0D992245C102}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17464,10 +18254,10 @@
         <v>62</v>
       </c>
       <c r="B2">
-        <v>627</v>
+        <v>679</v>
       </c>
       <c r="C2" s="1">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -17475,10 +18265,10 @@
         <v>61</v>
       </c>
       <c r="B3">
-        <v>711</v>
+        <v>797</v>
       </c>
       <c r="C3" s="1">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -17489,7 +18279,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="1">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -17497,10 +18287,10 @@
         <v>62</v>
       </c>
       <c r="B5">
-        <v>589</v>
+        <v>627</v>
       </c>
       <c r="C5" s="1">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -17508,10 +18298,10 @@
         <v>61</v>
       </c>
       <c r="B6">
-        <v>665</v>
+        <v>711</v>
       </c>
       <c r="C6" s="1">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -17522,7 +18312,7 @@
         <v>1</v>
       </c>
       <c r="C7" s="1">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -17530,10 +18320,10 @@
         <v>62</v>
       </c>
       <c r="B8">
-        <v>544</v>
+        <v>589</v>
       </c>
       <c r="C8" s="1">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -17541,10 +18331,10 @@
         <v>61</v>
       </c>
       <c r="B9">
-        <v>613</v>
+        <v>665</v>
       </c>
       <c r="C9" s="1">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -17555,7 +18345,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="1">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -17563,10 +18353,10 @@
         <v>62</v>
       </c>
       <c r="B11">
-        <v>441</v>
+        <v>544</v>
       </c>
       <c r="C11" s="1">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -17574,10 +18364,10 @@
         <v>61</v>
       </c>
       <c r="B12">
-        <v>462</v>
+        <v>613</v>
       </c>
       <c r="C12" s="1">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -17588,7 +18378,7 @@
         <v>1</v>
       </c>
       <c r="C13" s="1">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -17596,10 +18386,10 @@
         <v>62</v>
       </c>
       <c r="B14">
-        <v>384</v>
+        <v>441</v>
       </c>
       <c r="C14" s="1">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -17607,10 +18397,10 @@
         <v>61</v>
       </c>
       <c r="B15">
-        <v>389</v>
+        <v>462</v>
       </c>
       <c r="C15" s="1">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -17621,7 +18411,7 @@
         <v>1</v>
       </c>
       <c r="C16" s="1">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -17629,31 +18419,64 @@
         <v>62</v>
       </c>
       <c r="B17">
-        <v>342</v>
+        <v>384</v>
       </c>
       <c r="C17" s="1">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>61</v>
       </c>
       <c r="B18">
-        <v>347</v>
+        <v>389</v>
       </c>
       <c r="C18" s="1">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>52</v>
       </c>
-      <c r="B19" t="s">
-        <v>8</v>
+      <c r="B19">
+        <v>1</v>
       </c>
       <c r="C19" s="1">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>62</v>
+      </c>
+      <c r="B20">
+        <v>342</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21">
+        <v>347</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>52</v>
+      </c>
+      <c r="B22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C22" s="1">
         <v>43922</v>
       </c>
     </row>
@@ -17664,10 +18487,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD393D6-56CC-E749-BDF2-72DC274BB8BB}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17688,10 +18511,10 @@
         <v>143</v>
       </c>
       <c r="B2">
-        <v>431</v>
+        <v>467</v>
       </c>
       <c r="C2" s="1">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -17699,10 +18522,10 @@
         <v>144</v>
       </c>
       <c r="B3">
-        <v>522</v>
+        <v>569</v>
       </c>
       <c r="C3" s="1">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -17710,10 +18533,10 @@
         <v>145</v>
       </c>
       <c r="B4">
-        <v>386</v>
+        <v>441</v>
       </c>
       <c r="C4" s="1">
-        <v>43929</v>
+        <v>43930</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -17721,10 +18544,10 @@
         <v>143</v>
       </c>
       <c r="B5">
-        <v>408</v>
+        <v>431</v>
       </c>
       <c r="C5" s="1">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -17732,10 +18555,10 @@
         <v>144</v>
       </c>
       <c r="B6">
-        <v>487</v>
+        <v>522</v>
       </c>
       <c r="C6" s="1">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -17743,10 +18566,10 @@
         <v>145</v>
       </c>
       <c r="B7">
-        <v>360</v>
+        <v>386</v>
       </c>
       <c r="C7" s="1">
-        <v>43928</v>
+        <v>43929</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -17754,10 +18577,10 @@
         <v>143</v>
       </c>
       <c r="B8">
-        <v>370</v>
+        <v>408</v>
       </c>
       <c r="C8" s="1">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -17765,10 +18588,10 @@
         <v>144</v>
       </c>
       <c r="B9">
-        <v>458</v>
+        <v>487</v>
       </c>
       <c r="C9" s="1">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -17776,10 +18599,10 @@
         <v>145</v>
       </c>
       <c r="B10">
-        <v>330</v>
+        <v>360</v>
       </c>
       <c r="C10" s="1">
-        <v>43927</v>
+        <v>43928</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -17787,10 +18610,10 @@
         <v>143</v>
       </c>
       <c r="B11">
-        <v>286</v>
+        <v>370</v>
       </c>
       <c r="C11" s="1">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -17798,10 +18621,10 @@
         <v>144</v>
       </c>
       <c r="B12">
-        <v>362</v>
+        <v>458</v>
       </c>
       <c r="C12" s="1">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -17809,10 +18632,10 @@
         <v>145</v>
       </c>
       <c r="B13">
-        <v>256</v>
+        <v>330</v>
       </c>
       <c r="C13" s="1">
-        <v>43924</v>
+        <v>43927</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -17820,10 +18643,10 @@
         <v>143</v>
       </c>
       <c r="B14">
-        <v>249</v>
+        <v>286</v>
       </c>
       <c r="C14" s="1">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -17831,10 +18654,10 @@
         <v>144</v>
       </c>
       <c r="B15">
-        <v>307</v>
+        <v>362</v>
       </c>
       <c r="C15" s="1">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
@@ -17842,10 +18665,10 @@
         <v>145</v>
       </c>
       <c r="B16">
-        <v>218</v>
+        <v>256</v>
       </c>
       <c r="C16" s="1">
-        <v>43923</v>
+        <v>43924</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
@@ -17853,10 +18676,10 @@
         <v>143</v>
       </c>
       <c r="B17">
-        <v>223</v>
+        <v>249</v>
       </c>
       <c r="C17" s="1">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
@@ -17864,10 +18687,10 @@
         <v>144</v>
       </c>
       <c r="B18">
-        <v>271</v>
+        <v>307</v>
       </c>
       <c r="C18" s="1">
-        <v>43922</v>
+        <v>43923</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
@@ -17875,9 +18698,42 @@
         <v>145</v>
       </c>
       <c r="B19">
+        <v>218</v>
+      </c>
+      <c r="C19" s="1">
+        <v>43923</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>143</v>
+      </c>
+      <c r="B20">
+        <v>223</v>
+      </c>
+      <c r="C20" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B21">
+        <v>271</v>
+      </c>
+      <c r="C21" s="1">
+        <v>43922</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>145</v>
+      </c>
+      <c r="B22">
         <v>195</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C22" s="1">
         <v>43922</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated data and minor UI change
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DCE53F-E742-B045-9C34-2D30699852CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB948F14-42EA-684E-8741-C97281BBB036}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -981,7 +981,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -998,6 +998,7 @@
     <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1354,15 +1355,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5E2DA3-023C-FF46-A014-0C2E672468A0}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="15.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -1374,12 +1375,15 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="1">
-        <v>43927</v>
-      </c>
-      <c r="B2" s="1">
-        <v>43930</v>
-      </c>
+      <c r="A2" s="12">
+        <v>43928.817847222221</v>
+      </c>
+      <c r="B2" s="12">
+        <v>43930.81794375</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Fixed to manually scrape NI data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B77FFC8-0928-D340-A7A4-18CFD19A1A9F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9792821E-95F0-8845-B1CB-263D8D5DB5CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14400" yWindow="460" windowWidth="14400" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16160" firstSheet="5" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1642" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1643" uniqueCount="152">
   <si>
     <t>Date</t>
   </si>
@@ -493,6 +493,9 @@
   </si>
   <si>
     <t>https://www.gov.ie/en/news/7e0924-latest-updates-on-covid-19-coronavirus/</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -1360,7 +1363,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5E2DA3-023C-FF46-A014-0C2E672468A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1380,11 +1383,11 @@
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
         <f ca="1">NOW()-3</f>
-        <v>43928.791318750002</v>
+        <v>43928.794707754627</v>
       </c>
       <c r="B2" s="12">
         <f ca="1">NOW()</f>
-        <v>43931.791318750002</v>
+        <v>43931.794707754627</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1397,875 +1400,1025 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C39AE50F-07C0-7048-95B5-0C81D93B81F0}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C91"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B85" sqref="B85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="2" max="2" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="8">
+      <c r="C2" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C4" s="8">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C5" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C6" s="8">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C7" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C9" s="8">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B10" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>43922</v>
+      </c>
+      <c r="B12" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C12" s="8">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B13" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="8">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B15" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C15" s="8">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B16" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C16" s="8">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C17" s="8">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B18" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C18" s="8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C19" s="8">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C20" s="8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C21" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B22" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C22" s="8">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>43923</v>
+      </c>
+      <c r="B23" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="C23" s="8">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B24" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C24" s="8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C25" s="8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B26" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C26" s="8">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C27" s="8">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B28" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C28" s="8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B29" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C29" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B30" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C30" s="8">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" s="8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C32" s="8">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C33" s="8">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>43924</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C34" s="8">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C35" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C36" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C37" s="8">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" s="8">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" s="8">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="8">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C41" s="8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C42" s="8">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C43" s="8">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" s="8">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>43927</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" s="8">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C46" s="8">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" s="8">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C48" s="8">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C49" s="8">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C50" s="8">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C51" s="8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A52" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C52" s="8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A53" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C53" s="8">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A54" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C54" s="8">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A55" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C55" s="8">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A56" s="9">
+        <v>43928</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C56" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A57" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C57" s="8">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A58" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="C58" s="8">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A59" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="C59" s="8">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A60" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>121</v>
+      </c>
+      <c r="C60" s="8">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A61" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="C61" s="8">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A62" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B62" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="C62" s="8">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A63" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B63" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="C63" s="8">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A64" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="C64" s="8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A65" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B65" s="8" t="s">
+        <v>126</v>
+      </c>
+      <c r="C65" s="8">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A66" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B66" s="8" t="s">
+        <v>127</v>
+      </c>
+      <c r="C66" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A67" s="9">
+        <v>43929</v>
+      </c>
+      <c r="B67" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="C67" s="8">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A68" s="9">
+        <v>43930</v>
+      </c>
+      <c r="B68" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="C68" s="8">
         <v>89</v>
       </c>
-      <c r="C2" s="9">
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A69" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
+      <c r="B69" s="8" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="8">
+      <c r="C69" s="8">
         <v>120</v>
       </c>
-      <c r="C3" s="9">
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="B70" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="B4" s="8">
+      <c r="C70" s="8">
         <v>142</v>
       </c>
-      <c r="C4" s="9">
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
+      <c r="B71" s="8" t="s">
         <v>121</v>
       </c>
-      <c r="B5" s="8">
+      <c r="C71" s="8">
         <v>482</v>
       </c>
-      <c r="C5" s="9">
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
+      <c r="B72" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="B6" s="8">
+      <c r="C72" s="8">
         <v>43</v>
       </c>
-      <c r="C6" s="9">
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
+      <c r="B73" s="8" t="s">
         <v>123</v>
       </c>
-      <c r="B7" s="8">
+      <c r="C73" s="8">
         <v>52</v>
       </c>
-      <c r="C7" s="9">
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="8" t="s">
+      <c r="B74" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="B8" s="8">
+      <c r="C74" s="8">
         <v>43</v>
       </c>
-      <c r="C8" s="9">
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="8" t="s">
+      <c r="B75" s="8" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="8">
+      <c r="C75" s="8">
         <v>164</v>
       </c>
-      <c r="C9" s="9">
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="8" t="s">
+      <c r="B76" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B10" s="8">
+      <c r="C76" s="8">
         <v>80</v>
       </c>
-      <c r="C10" s="9">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="8" t="s">
+      <c r="B77" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="B11" s="8">
+      <c r="C77" s="8">
         <v>53</v>
       </c>
-      <c r="C11" s="9">
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" s="9">
         <v>43930</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="8" t="s">
+      <c r="B78" s="8" t="s">
         <v>128</v>
       </c>
-      <c r="B12" s="8">
+      <c r="C78" s="8">
         <v>92</v>
       </c>
-      <c r="C12" s="9">
-        <v>43930</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B13" s="8">
-        <v>81</v>
-      </c>
-      <c r="C13" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B14" s="8">
-        <v>110</v>
-      </c>
-      <c r="C14" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B15" s="8">
-        <v>135</v>
-      </c>
-      <c r="C15" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B16" s="8">
-        <v>429</v>
-      </c>
-      <c r="C16" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B17" s="8">
-        <v>35</v>
-      </c>
-      <c r="C17" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B18" s="8">
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <f>A68+1</f>
+        <v>43931</v>
+      </c>
+      <c r="B79" t="str">
+        <f>B68</f>
+        <v>Antrim And Newtownabbey</v>
+      </c>
+      <c r="C79" s="8">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <f t="shared" ref="A80:A91" si="0">A69+1</f>
+        <v>43931</v>
+      </c>
+      <c r="B80" t="str">
+        <f t="shared" ref="B80:B91" si="1">B69</f>
+        <v>Ards And North Down</v>
+      </c>
+      <c r="C80" s="8">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B81" t="str">
+        <f t="shared" si="1"/>
+        <v>Armagh, Banbridge And Craigavon</v>
+      </c>
+      <c r="C81" s="8">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B82" t="str">
+        <f t="shared" si="1"/>
+        <v>Belfast</v>
+      </c>
+      <c r="C82" s="8">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B83" t="str">
+        <f t="shared" si="1"/>
+        <v>Causeway Coast And Glens</v>
+      </c>
+      <c r="C83" s="8">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B84" t="str">
+        <f t="shared" si="1"/>
+        <v>Derry And Strabane</v>
+      </c>
+      <c r="C84" s="8">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B85" t="str">
+        <f t="shared" si="1"/>
+        <v>Fermanagh And Omagh</v>
+      </c>
+      <c r="C85" s="8">
         <v>52</v>
       </c>
-      <c r="C18" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B19" s="8">
-        <v>43</v>
-      </c>
-      <c r="C19" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" s="8">
-        <v>150</v>
-      </c>
-      <c r="C20" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B21" s="8">
-        <v>70</v>
-      </c>
-      <c r="C21" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B22" s="8">
-        <v>47</v>
-      </c>
-      <c r="C22" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B23" s="8">
-        <v>82</v>
-      </c>
-      <c r="C23" s="9">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B24" s="8">
-        <v>78</v>
-      </c>
-      <c r="C24" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B25" s="8">
-        <v>105</v>
-      </c>
-      <c r="C25" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B26" s="8">
-        <v>120</v>
-      </c>
-      <c r="C26" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B27" s="8">
-        <v>396</v>
-      </c>
-      <c r="C27" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B28" s="8">
-        <v>32</v>
-      </c>
-      <c r="C28" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B29" s="8">
-        <v>52</v>
-      </c>
-      <c r="C29" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B30" s="8">
-        <v>43</v>
-      </c>
-      <c r="C30" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B31" s="8">
-        <v>143</v>
-      </c>
-      <c r="C31" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B32" s="8">
-        <v>69</v>
-      </c>
-      <c r="C32" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B33" s="8">
-        <v>42</v>
-      </c>
-      <c r="C33" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B34" s="8">
-        <v>80</v>
-      </c>
-      <c r="C34" s="9">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B35" s="8">
-        <v>70</v>
-      </c>
-      <c r="C35" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B36" s="8">
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B86" t="str">
+        <f t="shared" si="1"/>
+        <v>Lisburn And Castlereagh</v>
+      </c>
+      <c r="C86" s="8">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B87" t="str">
+        <f t="shared" si="1"/>
+        <v>Mid And East Antrim</v>
+      </c>
+      <c r="C87" s="8">
         <v>102</v>
       </c>
-      <c r="C36" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B37" s="8">
-        <v>109</v>
-      </c>
-      <c r="C37" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B38" s="8">
-        <v>377</v>
-      </c>
-      <c r="C38" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B39" s="8">
-        <v>26</v>
-      </c>
-      <c r="C39" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B40" s="8">
-        <v>51</v>
-      </c>
-      <c r="C40" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B41" s="8">
-        <v>42</v>
-      </c>
-      <c r="C41" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B42" s="8">
-        <v>130</v>
-      </c>
-      <c r="C42" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B43" s="8">
-        <v>59</v>
-      </c>
-      <c r="C43" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B44" s="8">
-        <v>33</v>
-      </c>
-      <c r="C44" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B45" s="8">
-        <v>76</v>
-      </c>
-      <c r="C45" s="9">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B46" s="8">
-        <v>59</v>
-      </c>
-      <c r="C46" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="8" t="s">
-        <v>119</v>
-      </c>
-      <c r="B47" s="8">
-        <v>81</v>
-      </c>
-      <c r="C47" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B48" s="8">
-        <v>91</v>
-      </c>
-      <c r="C48" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B49" s="8">
-        <v>272</v>
-      </c>
-      <c r="C49" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B50" s="8">
-        <v>21</v>
-      </c>
-      <c r="C50" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B51" s="8">
-        <v>35</v>
-      </c>
-      <c r="C51" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B52" s="8">
-        <v>40</v>
-      </c>
-      <c r="C52" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B53" s="8">
-        <v>109</v>
-      </c>
-      <c r="C53" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B54" s="8">
-        <v>46</v>
-      </c>
-      <c r="C54" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B55" s="8">
-        <v>23</v>
-      </c>
-      <c r="C55" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B56" s="8">
-        <v>61</v>
-      </c>
-      <c r="C56" s="9">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B57" s="8">
-        <v>51</v>
-      </c>
-      <c r="C57" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B58" s="8">
-        <v>79</v>
-      </c>
-      <c r="C58" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B59" s="8">
-        <v>226</v>
-      </c>
-      <c r="C59" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B60" s="8">
-        <v>19</v>
-      </c>
-      <c r="C60" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B61" s="8">
-        <v>30</v>
-      </c>
-      <c r="C61" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B62" s="8">
-        <v>37</v>
-      </c>
-      <c r="C62" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B63" s="8">
-        <v>97</v>
-      </c>
-      <c r="C63" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B64" s="8">
-        <v>37</v>
-      </c>
-      <c r="C64" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" s="8">
-        <v>21</v>
-      </c>
-      <c r="C65" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="8">
-        <v>55</v>
-      </c>
-      <c r="C66" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" s="8">
-        <v>75</v>
-      </c>
-      <c r="C67" s="9">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="8" t="s">
-        <v>118</v>
-      </c>
-      <c r="B68" s="8">
-        <v>47</v>
-      </c>
-      <c r="C68" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="8" t="s">
-        <v>120</v>
-      </c>
-      <c r="B69" s="8">
-        <v>70</v>
-      </c>
-      <c r="C69" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="B70" s="8">
-        <v>200</v>
-      </c>
-      <c r="C70" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="B71" s="8">
-        <v>18</v>
-      </c>
-      <c r="C71" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="8" t="s">
-        <v>123</v>
-      </c>
-      <c r="B72" s="8">
-        <v>29</v>
-      </c>
-      <c r="C72" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="8" t="s">
-        <v>124</v>
-      </c>
-      <c r="B73" s="8">
-        <v>32</v>
-      </c>
-      <c r="C73" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="8" t="s">
-        <v>125</v>
-      </c>
-      <c r="B74" s="8">
-        <v>81</v>
-      </c>
-      <c r="C74" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="8" t="s">
-        <v>126</v>
-      </c>
-      <c r="B75" s="8">
-        <v>36</v>
-      </c>
-      <c r="C75" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="8" t="s">
-        <v>127</v>
-      </c>
-      <c r="B76" s="8">
-        <v>19</v>
-      </c>
-      <c r="C76" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B77" s="8">
-        <v>51</v>
-      </c>
-      <c r="C77" s="9">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="B78" s="8">
-        <v>67</v>
-      </c>
-      <c r="C78" s="9">
-        <v>43922</v>
-      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B88" t="str">
+        <f t="shared" si="1"/>
+        <v>Mid Ulster</v>
+      </c>
+      <c r="C88" s="8">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B89" t="str">
+        <f t="shared" si="1"/>
+        <v>Newry, Mourne And Down</v>
+      </c>
+      <c r="C89" s="8">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" s="1"/>
+      <c r="C90" s="8"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -18020,10 +18173,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE73A96-9009-C14A-A4D6-627BDCEBA7A8}">
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18056,98 +18209,98 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
-        <v>43930</v>
+        <v>43922</v>
       </c>
       <c r="B2">
-        <v>138</v>
+        <v>103</v>
       </c>
       <c r="C2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D2">
-        <v>1477</v>
+        <v>689</v>
       </c>
       <c r="E2">
-        <v>82</v>
+        <v>30</v>
       </c>
       <c r="F2">
-        <v>10203</v>
+        <v>6450</v>
       </c>
       <c r="G2" s="10">
         <f>D2/F2</f>
-        <v>0.14476134470253846</v>
+        <v>0.10682170542635659</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>43929</v>
+        <v>43923</v>
       </c>
       <c r="B3">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="C3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D3">
-        <v>1339</v>
+        <v>774</v>
       </c>
       <c r="E3">
-        <v>78</v>
+        <v>36</v>
       </c>
       <c r="F3">
-        <v>9564</v>
+        <v>6899</v>
       </c>
       <c r="G3" s="10">
         <f>D3/F3</f>
-        <v>0.14000418235048098</v>
+        <v>0.11219017248876649</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>43928</v>
+        <v>43924</v>
       </c>
       <c r="B4">
-        <v>97</v>
+        <v>130</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="D4">
-        <v>1255</v>
+        <v>904</v>
       </c>
       <c r="E4">
-        <v>73</v>
+        <v>48</v>
       </c>
       <c r="F4">
-        <v>9158</v>
+        <v>7525</v>
       </c>
       <c r="G4" s="10">
-        <f t="shared" ref="G4:G10" si="0">D4/F4</f>
-        <v>0.13703865472810658</v>
+        <f>D4/F4</f>
+        <v>0.12013289036544851</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>43927</v>
+        <v>43925</v>
       </c>
       <c r="B5">
-        <v>69</v>
+        <v>94</v>
       </c>
       <c r="C5">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D5">
-        <v>1158</v>
+        <v>998</v>
       </c>
       <c r="E5">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="F5">
-        <v>8740</v>
+        <v>8034</v>
       </c>
       <c r="G5" s="10">
-        <f t="shared" si="0"/>
-        <v>0.13249427917620138</v>
+        <f>D5/F5</f>
+        <v>0.12422205626089121</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -18170,361 +18323,427 @@
         <v>8486</v>
       </c>
       <c r="G6" s="10">
-        <f t="shared" si="0"/>
+        <f>D6/F6</f>
         <v>0.12832901249116191</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>43925</v>
+        <v>43927</v>
       </c>
       <c r="B7">
-        <v>94</v>
+        <v>69</v>
       </c>
       <c r="C7">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D7">
-        <v>998</v>
+        <v>1158</v>
       </c>
       <c r="E7">
-        <v>56</v>
+        <v>70</v>
       </c>
       <c r="F7">
-        <v>8034</v>
+        <v>8740</v>
       </c>
       <c r="G7" s="10">
-        <f t="shared" si="0"/>
-        <v>0.12422205626089121</v>
+        <f>D7/F7</f>
+        <v>0.13249427917620138</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>43924</v>
+        <v>43928</v>
       </c>
       <c r="B8">
-        <v>130</v>
+        <v>97</v>
       </c>
       <c r="C8">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="D8">
-        <v>904</v>
+        <v>1255</v>
       </c>
       <c r="E8">
-        <v>48</v>
+        <v>73</v>
       </c>
       <c r="F8">
-        <v>7525</v>
+        <v>9158</v>
       </c>
       <c r="G8" s="10">
-        <f t="shared" si="0"/>
-        <v>0.12013289036544851</v>
+        <f>D8/F8</f>
+        <v>0.13703865472810658</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>43923</v>
+        <v>43929</v>
       </c>
       <c r="B9">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D9">
-        <v>774</v>
+        <v>1339</v>
       </c>
       <c r="E9">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="F9">
-        <v>6899</v>
+        <v>9564</v>
       </c>
       <c r="G9" s="10">
-        <f t="shared" si="0"/>
-        <v>0.11219017248876649</v>
+        <f>D9/F9</f>
+        <v>0.14000418235048098</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>43922</v>
+        <v>43930</v>
       </c>
       <c r="B10">
-        <v>103</v>
+        <v>138</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D10">
-        <v>689</v>
+        <v>1477</v>
       </c>
       <c r="E10">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="F10">
-        <v>6450</v>
+        <v>10203</v>
       </c>
       <c r="G10" s="10">
-        <f t="shared" si="0"/>
-        <v>0.10682170542635659</v>
+        <f>D10/F10</f>
+        <v>0.14476134470253846</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43931</v>
+      </c>
+      <c r="B11">
+        <v>112</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+      <c r="D11">
+        <v>1589</v>
+      </c>
+      <c r="E11">
+        <v>92</v>
+      </c>
+      <c r="F11">
+        <v>11006</v>
+      </c>
+      <c r="G11" s="10">
+        <f>D11/F11</f>
+        <v>0.1443757950208977</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G10">
+    <sortCondition ref="A2:A10"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0979910-C687-6A43-A609-0D992245C102}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>140</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>141</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B2" t="s">
         <v>62</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B3" t="s">
+        <v>61</v>
+      </c>
+      <c r="C3">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C5">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C8">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C9">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B11" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B12" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B13" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B14" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C15">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B17" t="s">
+        <v>62</v>
+      </c>
+      <c r="C17">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B19" t="s">
+        <v>52</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C20">
         <v>679</v>
       </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>43930</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B21" t="s">
         <v>61</v>
       </c>
-      <c r="B3">
+      <c r="C21">
         <v>797</v>
       </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>43930</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="B4">
+      <c r="C22">
         <v>1</v>
       </c>
-      <c r="C4" s="1">
-        <v>43930</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>62</v>
-      </c>
-      <c r="B5">
-        <v>627</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B6">
-        <v>711</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>52</v>
-      </c>
-      <c r="B7">
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f>A20+1</f>
+        <v>43931</v>
+      </c>
+      <c r="B23" t="str">
+        <f>B20</f>
+        <v>Male</v>
+      </c>
+      <c r="C23">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" ref="A24:A25" si="0">A21+1</f>
+        <v>43931</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" ref="B24:B25" si="1">B21</f>
+        <v>Female</v>
+      </c>
+      <c r="C24">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>Unknown</v>
+      </c>
+      <c r="C25">
         <v>1</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B8">
-        <v>589</v>
-      </c>
-      <c r="C8" s="1">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>61</v>
-      </c>
-      <c r="B9">
-        <v>665</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-      <c r="B10">
-        <v>1</v>
-      </c>
-      <c r="C10" s="1">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11">
-        <v>544</v>
-      </c>
-      <c r="C11" s="1">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12">
-        <v>613</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13">
-        <v>1</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14">
-        <v>441</v>
-      </c>
-      <c r="C14" s="1">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>61</v>
-      </c>
-      <c r="B15">
-        <v>462</v>
-      </c>
-      <c r="C15" s="1">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>52</v>
-      </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" s="1">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17">
-        <v>384</v>
-      </c>
-      <c r="C17" s="1">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>61</v>
-      </c>
-      <c r="B18">
-        <v>389</v>
-      </c>
-      <c r="C18" s="1">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>52</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" s="1">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>62</v>
-      </c>
-      <c r="B20">
-        <v>342</v>
-      </c>
-      <c r="C20" s="1">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>61</v>
-      </c>
-      <c r="B21">
-        <v>347</v>
-      </c>
-      <c r="C21" s="1">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>52</v>
-      </c>
-      <c r="B22" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="1">
-        <v>43922</v>
       </c>
     </row>
   </sheetData>
@@ -18534,254 +18753,298 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD393D6-56CC-E749-BDF2-72DC274BB8BB}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
         <v>142</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>141</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="A2" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B2" t="s">
         <v>143</v>
       </c>
-      <c r="B2">
+      <c r="C2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C3">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>43922</v>
+      </c>
+      <c r="B4" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C5">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B6" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>43923</v>
+      </c>
+      <c r="B7" t="s">
+        <v>145</v>
+      </c>
+      <c r="C7">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B8" t="s">
+        <v>143</v>
+      </c>
+      <c r="C8">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B9" t="s">
+        <v>144</v>
+      </c>
+      <c r="C9">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>43924</v>
+      </c>
+      <c r="B10" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B11" t="s">
+        <v>143</v>
+      </c>
+      <c r="C11">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B12" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>43927</v>
+      </c>
+      <c r="B13" t="s">
+        <v>145</v>
+      </c>
+      <c r="C13">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B14" t="s">
+        <v>143</v>
+      </c>
+      <c r="C14">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B15" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" s="1">
+        <v>43928</v>
+      </c>
+      <c r="B16" t="s">
+        <v>145</v>
+      </c>
+      <c r="C16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B17" t="s">
+        <v>143</v>
+      </c>
+      <c r="C17">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B18" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>43929</v>
+      </c>
+      <c r="B19" t="s">
+        <v>145</v>
+      </c>
+      <c r="C19">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B20" t="s">
+        <v>143</v>
+      </c>
+      <c r="C20">
         <v>467</v>
       </c>
-      <c r="C2" s="1">
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
         <v>43930</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B21" t="s">
         <v>144</v>
       </c>
-      <c r="B3">
+      <c r="C21">
         <v>569</v>
       </c>
-      <c r="C3" s="1">
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
         <v>43930</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B22" t="s">
         <v>145</v>
       </c>
-      <c r="B4">
+      <c r="C22">
         <v>441</v>
       </c>
-      <c r="C4" s="1">
-        <v>43930</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>143</v>
-      </c>
-      <c r="B5">
-        <v>431</v>
-      </c>
-      <c r="C5" s="1">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>144</v>
-      </c>
-      <c r="B6">
-        <v>522</v>
-      </c>
-      <c r="C6" s="1">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>145</v>
-      </c>
-      <c r="B7">
-        <v>386</v>
-      </c>
-      <c r="C7" s="1">
-        <v>43929</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>143</v>
-      </c>
-      <c r="B8">
-        <v>408</v>
-      </c>
-      <c r="C8" s="1">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>144</v>
-      </c>
-      <c r="B9">
-        <v>487</v>
-      </c>
-      <c r="C9" s="1">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>145</v>
-      </c>
-      <c r="B10">
-        <v>360</v>
-      </c>
-      <c r="C10" s="1">
-        <v>43928</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B11">
-        <v>370</v>
-      </c>
-      <c r="C11" s="1">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>144</v>
-      </c>
-      <c r="B12">
-        <v>458</v>
-      </c>
-      <c r="C12" s="1">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>145</v>
-      </c>
-      <c r="B13">
-        <v>330</v>
-      </c>
-      <c r="C13" s="1">
-        <v>43927</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>143</v>
-      </c>
-      <c r="B14">
-        <v>286</v>
-      </c>
-      <c r="C14" s="1">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>144</v>
-      </c>
-      <c r="B15">
-        <v>362</v>
-      </c>
-      <c r="C15" s="1">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16">
-        <v>256</v>
-      </c>
-      <c r="C16" s="1">
-        <v>43924</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>143</v>
-      </c>
-      <c r="B17">
-        <v>249</v>
-      </c>
-      <c r="C17" s="1">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>144</v>
-      </c>
-      <c r="B18">
-        <v>307</v>
-      </c>
-      <c r="C18" s="1">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>145</v>
-      </c>
-      <c r="B19">
-        <v>218</v>
-      </c>
-      <c r="C19" s="1">
-        <v>43923</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>143</v>
-      </c>
-      <c r="B20">
-        <v>223</v>
-      </c>
-      <c r="C20" s="1">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>144</v>
-      </c>
-      <c r="B21">
-        <v>271</v>
-      </c>
-      <c r="C21" s="1">
-        <v>43922</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>145</v>
-      </c>
-      <c r="B22">
-        <v>195</v>
-      </c>
-      <c r="C22" s="1">
-        <v>43922</v>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <f>A20+1</f>
+        <v>43931</v>
+      </c>
+      <c r="B23" t="str">
+        <f>B20</f>
+        <v>0_to_44</v>
+      </c>
+      <c r="C23">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <f t="shared" ref="A24:A25" si="0">A21+1</f>
+        <v>43931</v>
+      </c>
+      <c r="B24" t="str">
+        <f t="shared" ref="B24:B25" si="1">B21</f>
+        <v>45_to_69</v>
+      </c>
+      <c r="C24">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <f t="shared" si="0"/>
+        <v>43931</v>
+      </c>
+      <c r="B25" t="str">
+        <f t="shared" si="1"/>
+        <v>70+</v>
+      </c>
+      <c r="C25">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="C26" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated to latest data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27118C2B-E02B-E545-8B72-0FFFC6E0995E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{411E570D-F0D7-3F46-ADF0-D5DF185E52FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-20" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1681" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1720" uniqueCount="152">
   <si>
     <t>Date</t>
   </si>
@@ -486,19 +486,16 @@
     <t>Pos_prop</t>
   </si>
   <si>
-    <t>https://www.gov.ie/en/news/7e0924-latest-updates-on-covid-19-coronavirus/#april-9</t>
-  </si>
-  <si>
     <t>https://www.gov.ie/en/publication/695f10-an-analysis-of-the-6444-cases-of-covid-19-in-ireland-as-of-tuesday-7/</t>
   </si>
   <si>
     <t>https://www.gov.ie/en/news/7e0924-latest-updates-on-covid-19-coronavirus/</t>
   </si>
   <si>
-    <t>s</t>
+    <t>https://www.gov.ie/en/press-release/895657-statement-from-the-national-public-health-emergency-team-friday-10-a/</t>
   </si>
   <si>
-    <t>https://www.gov.ie/en/press-release/895657-statement-from-the-national-public-health-emergency-team-friday-10-a/</t>
+    <t>https://www.gov.ie/en/press-release/28cb70-statement-from-the-national-public-health-emergency-team-saturday-11/</t>
   </si>
 </sst>
 </file>
@@ -1367,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5E2DA3-023C-FF46-A014-0C2E672468A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1386,10 +1383,10 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12">
-        <v>43929.827473495374</v>
+        <v>43930.811111111114</v>
       </c>
       <c r="B2" s="12">
-        <v>43931.881249999999</v>
+        <v>43932.811111111114</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -1405,7 +1402,7 @@
   <dimension ref="A1:C91"/>
   <sheetViews>
     <sheetView topLeftCell="A57" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B85" sqref="B85"/>
+      <selection activeCell="C105" sqref="C105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2416,7 +2413,9 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="1"/>
+      <c r="A90" s="1">
+        <v>43932</v>
+      </c>
       <c r="C90" s="8"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
@@ -2557,7 +2556,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C33" sqref="C33"/>
+      <selection pane="bottomRight" activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3489,7 +3488,7 @@
         <v>4916</v>
       </c>
       <c r="D27" s="5">
-        <f t="shared" ref="D27:D33" si="0">C27-C26</f>
+        <f t="shared" ref="D27:D34" si="0">C27-C26</f>
         <v>473</v>
       </c>
       <c r="E27" s="5">
@@ -3619,7 +3618,7 @@
         <v>48</v>
       </c>
       <c r="K30" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -3655,7 +3654,7 @@
         <v>48</v>
       </c>
       <c r="K31" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -3663,35 +3662,35 @@
         <v>43930</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C32">
-        <v>6574</v>
+        <v>7787</v>
       </c>
       <c r="D32" s="5">
         <f t="shared" si="0"/>
-        <v>-497</v>
-      </c>
-      <c r="E32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F32" t="s">
-        <v>8</v>
+        <v>716</v>
+      </c>
+      <c r="E32">
+        <v>1718</v>
+      </c>
+      <c r="F32">
+        <v>253</v>
       </c>
       <c r="G32" s="5">
-        <v>263</v>
-      </c>
-      <c r="H32" t="s">
-        <v>8</v>
-      </c>
-      <c r="I32" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32" t="s">
-        <v>8</v>
+        <v>314</v>
+      </c>
+      <c r="H32">
+        <v>2141</v>
+      </c>
+      <c r="I32">
+        <v>356</v>
+      </c>
+      <c r="J32">
+        <v>48</v>
       </c>
       <c r="K32" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="17" x14ac:dyDescent="0.2">
@@ -3706,7 +3705,7 @@
       </c>
       <c r="D33" s="5">
         <f t="shared" si="0"/>
-        <v>1515</v>
+        <v>302</v>
       </c>
       <c r="E33" t="s">
         <v>8</v>
@@ -3727,11 +3726,29 @@
         <v>8</v>
       </c>
       <c r="K33" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="17" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>43932</v>
+      </c>
+      <c r="B34" s="6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C34" s="5">
+        <v>8928</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="0"/>
+        <v>839</v>
+      </c>
+      <c r="G34" s="5">
+        <v>320</v>
+      </c>
+      <c r="K34" t="s">
+        <v>151</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3740,10 +3757,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B646AB9-6DFD-6342-9B5D-CA852E35631D}">
-  <dimension ref="A1:D68"/>
+  <dimension ref="A1:D71"/>
   <sheetViews>
     <sheetView topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D69" sqref="D69"/>
+      <selection activeCell="A69" sqref="A69:A71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4683,7 +4700,7 @@
         <v>43929</v>
       </c>
       <c r="B67" t="str">
-        <f t="shared" ref="B67:B68" si="1">B64</f>
+        <f t="shared" ref="B67:B71" si="1">B64</f>
         <v>Male</v>
       </c>
       <c r="C67">
@@ -4707,6 +4724,51 @@
       </c>
       <c r="D68">
         <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B69" t="str">
+        <f>B66</f>
+        <v>Female</v>
+      </c>
+      <c r="C69">
+        <v>4212</v>
+      </c>
+      <c r="D69">
+        <v>54.1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B70" t="str">
+        <f t="shared" si="1"/>
+        <v>Male</v>
+      </c>
+      <c r="C70">
+        <v>3489</v>
+      </c>
+      <c r="D70">
+        <v>44.8</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B71" t="str">
+        <f t="shared" si="1"/>
+        <v>Unknown</v>
+      </c>
+      <c r="C71">
+        <v>86</v>
+      </c>
+      <c r="D71">
+        <v>1.1000000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -4716,11 +4778,11 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2CC04-F5BC-6741-A3F2-2661873C87D7}">
-  <dimension ref="A1:E259"/>
+  <dimension ref="A1:F270"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A239" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D251" sqref="D251"/>
+      <selection pane="bottomLeft" activeCell="F260" sqref="F260:I268"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -8318,7 +8380,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="257" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <f t="shared" si="0"/>
         <v>43929</v>
@@ -8333,7 +8395,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="258" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <f t="shared" si="0"/>
         <v>43929</v>
@@ -8348,7 +8410,7 @@
         <v>819</v>
       </c>
     </row>
-    <row r="259" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <f t="shared" si="0"/>
         <v>43929</v>
@@ -8360,6 +8422,163 @@
         <v>19</v>
       </c>
       <c r="D259">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="260" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A260" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B260" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C260">
+        <v>18</v>
+      </c>
+      <c r="D260" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="261" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A261" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B261" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C261">
+        <v>22</v>
+      </c>
+      <c r="D261" t="s">
+        <v>8</v>
+      </c>
+      <c r="F261" s="7"/>
+    </row>
+    <row r="262" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A262" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B262" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C262" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D262">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="263" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B263" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C263">
+        <v>52</v>
+      </c>
+      <c r="D263">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="264" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A264" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B264" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C264">
+        <v>473</v>
+      </c>
+      <c r="D264">
+        <v>41</v>
+      </c>
+      <c r="E264" s="13"/>
+    </row>
+    <row r="265" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B265" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C265">
+        <v>1343</v>
+      </c>
+      <c r="D265">
+        <v>119</v>
+      </c>
+      <c r="E265" s="7"/>
+    </row>
+    <row r="266" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B266" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C266">
+        <v>1418</v>
+      </c>
+      <c r="D266">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="267" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B267" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C267">
+        <v>1479</v>
+      </c>
+      <c r="D267">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="268" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B268" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C268">
+        <v>1138</v>
+      </c>
+      <c r="D268">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="269" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B269" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C269">
+        <v>1825</v>
+      </c>
+      <c r="D269">
+        <v>871</v>
+      </c>
+    </row>
+    <row r="270" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B270" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="C270">
+        <v>19</v>
+      </c>
+      <c r="D270">
         <v>2</v>
       </c>
     </row>
@@ -8370,11 +8589,11 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{029AF1D0-4AE1-A540-B628-AF7C84CE0F40}">
-  <dimension ref="A1:D88"/>
+  <dimension ref="A1:D91"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C89" sqref="C89"/>
+      <selection pane="bottomLeft" activeCell="B92" sqref="B92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9596,7 +9815,7 @@
         <v>43929</v>
       </c>
       <c r="B87" t="str">
-        <f t="shared" ref="B87:B88" si="1">B84</f>
+        <f t="shared" ref="B87:B91" si="1">B84</f>
         <v>Close contact with confirmed case</v>
       </c>
       <c r="C87" s="11">
@@ -9619,6 +9838,51 @@
         <v>9</v>
       </c>
       <c r="D88" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B89" t="str">
+        <f>B86</f>
+        <v>Community transmission</v>
+      </c>
+      <c r="C89" s="11">
+        <v>66</v>
+      </c>
+      <c r="D89" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B90" t="str">
+        <f t="shared" si="1"/>
+        <v>Close contact with confirmed case</v>
+      </c>
+      <c r="C90" s="11">
+        <v>26</v>
+      </c>
+      <c r="D90" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A91" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B91" t="str">
+        <f t="shared" si="1"/>
+        <v>Travel Abroad</v>
+      </c>
+      <c r="C91" s="11">
+        <v>8</v>
+      </c>
+      <c r="D91" t="s">
         <v>106</v>
       </c>
     </row>
@@ -9629,10 +9893,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77735C93-7ED9-C044-B61C-E23C86F44D03}">
-  <dimension ref="A1:E619"/>
+  <dimension ref="A1:E645"/>
   <sheetViews>
-    <sheetView topLeftCell="A582" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A594" sqref="A594:A619"/>
+    <sheetView topLeftCell="A606" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="A620" sqref="A620:A645"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18795,6 +19059,370 @@
         <v>3.4000000000000002E-2</v>
       </c>
     </row>
+    <row r="620" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A620" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B620" t="s">
+        <v>12</v>
+      </c>
+      <c r="C620">
+        <v>22</v>
+      </c>
+      <c r="D620" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="621" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A621" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B621" t="s">
+        <v>14</v>
+      </c>
+      <c r="C621">
+        <v>169</v>
+      </c>
+      <c r="D621" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="622" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A622" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B622" t="s">
+        <v>15</v>
+      </c>
+      <c r="C622">
+        <v>85</v>
+      </c>
+      <c r="D622" s="3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="623" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A623" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B623" t="s">
+        <v>16</v>
+      </c>
+      <c r="C623">
+        <v>581</v>
+      </c>
+      <c r="D623" s="3">
+        <v>7.4999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="624" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A624" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B624" t="s">
+        <v>17</v>
+      </c>
+      <c r="C624">
+        <v>167</v>
+      </c>
+      <c r="D624" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="625" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A625" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B625" t="s">
+        <v>18</v>
+      </c>
+      <c r="C625">
+        <v>34156</v>
+      </c>
+      <c r="D625" s="3">
+        <v>0.53400000000000003</v>
+      </c>
+    </row>
+    <row r="626" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A626" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B626" t="s">
+        <v>19</v>
+      </c>
+      <c r="C626">
+        <v>169</v>
+      </c>
+      <c r="D626" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="627" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A627" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B627" t="s">
+        <v>20</v>
+      </c>
+      <c r="C627">
+        <v>155</v>
+      </c>
+      <c r="D627" s="2">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="628" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A628" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B628" t="s">
+        <v>21</v>
+      </c>
+      <c r="C628">
+        <v>332</v>
+      </c>
+      <c r="D628" s="3">
+        <v>4.2999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="629" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A629" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B629" t="s">
+        <v>22</v>
+      </c>
+      <c r="C629">
+        <v>115</v>
+      </c>
+      <c r="D629" s="3">
+        <v>1.4E-2</v>
+      </c>
+    </row>
+    <row r="630" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A630" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B630" t="s">
+        <v>36</v>
+      </c>
+      <c r="C630">
+        <v>61</v>
+      </c>
+      <c r="D630" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="631" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A631" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B631" t="s">
+        <v>37</v>
+      </c>
+      <c r="C631">
+        <v>31</v>
+      </c>
+      <c r="D631" s="3">
+        <v>4.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="632" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A632" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B632" t="s">
+        <v>23</v>
+      </c>
+      <c r="C632">
+        <v>222</v>
+      </c>
+      <c r="D632" s="3">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="633" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A633" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B633" t="s">
+        <v>24</v>
+      </c>
+      <c r="C633">
+        <v>45</v>
+      </c>
+      <c r="D633" s="3">
+        <v>6.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="634" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A634" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B634" t="s">
+        <v>25</v>
+      </c>
+      <c r="C634">
+        <v>133</v>
+      </c>
+      <c r="D634" s="3">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="635" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A635" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B635" t="s">
+        <v>26</v>
+      </c>
+      <c r="C635">
+        <v>168</v>
+      </c>
+      <c r="D635" s="3">
+        <v>2.1999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="636" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A636" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B636" t="s">
+        <v>27</v>
+      </c>
+      <c r="C636">
+        <v>230</v>
+      </c>
+      <c r="D636" s="2">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="637" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A637" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B637" t="s">
+        <v>38</v>
+      </c>
+      <c r="C637">
+        <v>81</v>
+      </c>
+      <c r="D637" s="2">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="638" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A638" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B638" t="s">
+        <v>28</v>
+      </c>
+      <c r="C638">
+        <v>104</v>
+      </c>
+      <c r="D638" s="3">
+        <v>1.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="639" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A639" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B639" t="s">
+        <v>29</v>
+      </c>
+      <c r="C639">
+        <v>27</v>
+      </c>
+      <c r="D639" s="3">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="640" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A640" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B640" t="s">
+        <v>30</v>
+      </c>
+      <c r="C640">
+        <v>39</v>
+      </c>
+      <c r="D640" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="641" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A641" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B641" t="s">
+        <v>31</v>
+      </c>
+      <c r="C641">
+        <v>1166</v>
+      </c>
+      <c r="D641" s="3">
+        <v>2.1000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="642" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A642" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B642" t="s">
+        <v>32</v>
+      </c>
+      <c r="C642">
+        <v>63</v>
+      </c>
+      <c r="D642" s="3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+    </row>
+    <row r="643" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A643" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B643" t="s">
+        <v>33</v>
+      </c>
+      <c r="C643">
+        <v>181</v>
+      </c>
+      <c r="D643" s="3">
+        <v>2.3E-2</v>
+      </c>
+    </row>
+    <row r="644" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A644" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B644" t="s">
+        <v>34</v>
+      </c>
+      <c r="C644">
+        <v>39</v>
+      </c>
+      <c r="D644" s="3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="645" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A645" s="1">
+        <v>43930</v>
+      </c>
+      <c r="B645" t="s">
+        <v>35</v>
+      </c>
+      <c r="C645">
+        <v>246</v>
+      </c>
+      <c r="D645" s="3">
+        <v>3.2000000000000001E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18802,10 +19430,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE73A96-9009-C14A-A4D6-627BDCEBA7A8}">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18856,7 +19484,7 @@
         <v>6450</v>
       </c>
       <c r="G2" s="10">
-        <f t="shared" ref="G2:G11" si="0">D2/F2</f>
+        <f t="shared" ref="G2:G12" si="0">D2/F2</f>
         <v>0.10682170542635659</v>
       </c>
     </row>
@@ -19074,6 +19702,30 @@
       <c r="G11" s="10">
         <f t="shared" si="0"/>
         <v>0.1443757950208977</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12" s="1">
+        <v>43932</v>
+      </c>
+      <c r="B12">
+        <v>128</v>
+      </c>
+      <c r="C12">
+        <v>15</v>
+      </c>
+      <c r="D12">
+        <v>1717</v>
+      </c>
+      <c r="E12">
+        <v>107</v>
+      </c>
+      <c r="F12">
+        <v>11765</v>
+      </c>
+      <c r="G12" s="10">
+        <f t="shared" si="0"/>
+        <v>0.14594135146621334</v>
       </c>
     </row>
   </sheetData>
@@ -19086,13 +19738,16 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0979910-C687-6A43-A609-0D992245C102}">
-  <dimension ref="A1:C25"/>
+  <dimension ref="A1:C28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -19355,7 +20010,7 @@
         <v>43931</v>
       </c>
       <c r="B24" t="str">
-        <f t="shared" ref="B24:B25" si="1">B21</f>
+        <f t="shared" ref="B24:B28" si="1">B21</f>
         <v>Female</v>
       </c>
       <c r="C24">
@@ -19374,6 +20029,15 @@
       <c r="C25">
         <v>1</v>
       </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A26" s="1"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A27" s="1"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A28" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -19384,7 +20048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBD393D6-56CC-E749-BDF2-72DC274BB8BB}">
   <dimension ref="A1:C26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -19672,8 +20336,8 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="C26" t="s">
-        <v>151</v>
+      <c r="A26" s="1">
+        <v>43932</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed bug in dates
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED77F7F-85AD-C94F-8A21-A95F06736B45}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342B9086-E710-0643-A091-4497DB987C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16160" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -1370,7 +1370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5E2DA3-023C-FF46-A014-0C2E672468A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1392,7 +1392,7 @@
         <v>43933.86041666667</v>
       </c>
       <c r="B2" s="12">
-        <v>43936.86041666667</v>
+        <v>43935.86041666667</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
@@ -21391,7 +21391,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2FE73A96-9009-C14A-A4D6-627BDCEBA7A8}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Corrected mistake in gender data 5/4
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{342B9086-E710-0643-A091-4497DB987C94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B9C3509-7A9F-7F4A-B034-091A81302839}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="14400" windowHeight="16160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -1370,7 +1370,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5E2DA3-023C-FF46-A014-0C2E672468A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -3886,8 +3886,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B646AB9-6DFD-6342-9B5D-CA852E35631D}">
   <dimension ref="A1:D80"/>
   <sheetViews>
-    <sheetView topLeftCell="A60" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="D58" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4690,7 +4690,7 @@
         <v>2946</v>
       </c>
       <c r="D57">
-        <v>62.7</v>
+        <v>52.7</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fixed mistake in ICU
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewparnell/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6917A2B5-8696-9444-B200-25B5192E32F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1782BEB7-AEA7-0A43-B14E-97AEDCAD4AAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" firstSheet="5" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16220" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -3376,11 +3376,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K40"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="D26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K38" sqref="K38"/>
+      <selection pane="bottomRight" activeCell="F39" sqref="F39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4715,7 +4715,7 @@
         <v>2082</v>
       </c>
       <c r="F38">
-        <v>194</v>
+        <v>294</v>
       </c>
       <c r="G38" s="5">
         <v>521</v>
@@ -12439,7 +12439,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77735C93-7ED9-C044-B61C-E23C86F44D03}">
   <dimension ref="A1:E801"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A764" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A764" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A776" sqref="A776:A801"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Bug in hospital data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9B2D7C-5EF8-5D4B-8FEA-483F0FEE1D27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2C21CB-7CE3-9E40-9DDA-960628C3915B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -6192,9 +6192,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5B2CC04-F5BC-6741-A3F2-2661873C87D7}">
   <dimension ref="A1:F347"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A315" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D338" sqref="D338"/>
+      <selection pane="bottomLeft" activeCell="D347" sqref="D347"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -11077,7 +11077,7 @@
         <v>3094</v>
       </c>
       <c r="D346">
-        <v>114</v>
+        <v>1144</v>
       </c>
     </row>
     <row r="347" spans="1:4" x14ac:dyDescent="0.2">
@@ -26083,7 +26083,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0979910-C687-6A43-A609-0D992245C102}">
   <dimension ref="A1:C34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView topLeftCell="A17" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Included provisional death/case figures
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEF0CF57-6E7F-BB46-BD48-D7511250E84C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87E5B3CD-6230-844F-A573-DF25647F4D71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2421" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2381" uniqueCount="169">
   <si>
     <t>Date</t>
   </si>
@@ -545,6 +545,9 @@
   </si>
   <si>
     <t>Previous provisional deaths</t>
+  </si>
+  <si>
+    <t>Daily deaths</t>
   </si>
 </sst>
 </file>
@@ -3395,24 +3398,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M47"/>
+  <dimension ref="A1:N47"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B30" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B9" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D44" sqref="D44"/>
+      <selection pane="bottomRight" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" customWidth="1"/>
-    <col min="3" max="5" width="10.5" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" customWidth="1"/>
+    <col min="3" max="4" width="10.5" customWidth="1"/>
+    <col min="5" max="5" width="10.5" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" hidden="1" customWidth="1"/>
+    <col min="7" max="8" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="68" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" ht="68" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3441,19 +3446,22 @@
         <v>167</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>168</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="5" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>43900</v>
       </c>
@@ -3481,8 +3489,8 @@
       <c r="I2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J2" s="5" t="s">
-        <v>8</v>
+      <c r="J2" s="5">
+        <v>0</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>8</v>
@@ -3490,11 +3498,14 @@
       <c r="L2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="6">
         <v>43901</v>
       </c>
@@ -3522,8 +3533,9 @@
       <c r="I3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="5" t="s">
-        <v>8</v>
+      <c r="J3" s="5">
+        <f t="shared" ref="J2:J47" si="0">H3-H2</f>
+        <v>1</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>8</v>
@@ -3531,11 +3543,14 @@
       <c r="L3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M3" t="s">
+      <c r="M3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>43902</v>
       </c>
@@ -3563,8 +3578,9 @@
       <c r="I4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="5" t="s">
-        <v>8</v>
+      <c r="J4" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K4" s="5" t="s">
         <v>8</v>
@@ -3572,11 +3588,14 @@
       <c r="L4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N4" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="5" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>43903</v>
       </c>
@@ -3605,19 +3624,23 @@
         <v>8</v>
       </c>
       <c r="J5" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="5">
         <v>2</v>
-      </c>
-      <c r="K5" s="5" t="s">
-        <v>8</v>
       </c>
       <c r="L5" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>43904</v>
       </c>
@@ -3645,8 +3668,9 @@
       <c r="I6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J6" s="5" t="s">
-        <v>8</v>
+      <c r="J6" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="K6" s="5" t="s">
         <v>8</v>
@@ -3654,11 +3678,14 @@
       <c r="L6" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>43905</v>
       </c>
@@ -3686,8 +3713,9 @@
       <c r="I7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J7" s="5" t="s">
-        <v>8</v>
+      <c r="J7" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="K7" s="5" t="s">
         <v>8</v>
@@ -3695,11 +3723,14 @@
       <c r="L7" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M7" t="s">
+      <c r="M7" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>43906</v>
       </c>
@@ -3728,19 +3759,23 @@
         <v>8</v>
       </c>
       <c r="J8" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="5">
         <v>59</v>
       </c>
-      <c r="K8" s="5">
+      <c r="L8" s="5">
         <v>23</v>
       </c>
-      <c r="L8" s="5" t="s">
+      <c r="M8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="9" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>43907</v>
       </c>
@@ -3769,19 +3804,23 @@
         <v>8</v>
       </c>
       <c r="J9" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K9" s="5">
         <v>84</v>
       </c>
-      <c r="K9" s="5">
+      <c r="L9" s="5">
         <v>26</v>
       </c>
-      <c r="L9" s="5">
+      <c r="M9" s="5">
         <v>43</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="10" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>43908</v>
       </c>
@@ -3810,19 +3849,23 @@
         <v>8</v>
       </c>
       <c r="J10" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K10" s="5">
         <v>114</v>
       </c>
-      <c r="K10" s="5">
+      <c r="L10" s="5">
         <v>27</v>
       </c>
-      <c r="L10" s="5">
+      <c r="M10" s="5">
         <v>44</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="6">
         <v>43909</v>
       </c>
@@ -3851,19 +3894,23 @@
         <v>8</v>
       </c>
       <c r="J11" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
         <v>147</v>
       </c>
-      <c r="K11" s="5">
+      <c r="L11" s="5">
         <v>29</v>
       </c>
-      <c r="L11" s="5">
+      <c r="M11" s="5">
         <v>44</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="6">
         <v>43910</v>
       </c>
@@ -3892,19 +3939,23 @@
         <v>8</v>
       </c>
       <c r="J12" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K12" s="5">
         <v>159</v>
       </c>
-      <c r="K12" s="5">
+      <c r="L12" s="5">
         <v>35</v>
       </c>
-      <c r="L12" s="5">
+      <c r="M12" s="5">
         <v>44</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="13" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="6">
         <v>43911</v>
       </c>
@@ -3933,19 +3984,23 @@
         <v>8</v>
       </c>
       <c r="J13" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K13" s="5">
         <v>208</v>
       </c>
-      <c r="K13" s="5">
+      <c r="L13" s="5">
         <v>37</v>
       </c>
-      <c r="L13" s="5">
+      <c r="M13" s="5">
         <v>44</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="6">
         <v>43912</v>
       </c>
@@ -3974,19 +4029,23 @@
         <v>8</v>
       </c>
       <c r="J14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K14" s="5">
         <v>247</v>
       </c>
-      <c r="K14" s="5">
+      <c r="L14" s="5">
         <v>44</v>
       </c>
-      <c r="L14" s="5">
+      <c r="M14" s="5">
         <v>45</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="6">
         <v>43913</v>
       </c>
@@ -4015,19 +4074,23 @@
         <v>8</v>
       </c>
       <c r="J15" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K15" s="5">
         <v>283</v>
       </c>
-      <c r="K15" s="5">
+      <c r="L15" s="5">
         <v>63</v>
       </c>
-      <c r="L15" s="5">
+      <c r="M15" s="5">
         <v>45</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="6">
         <v>43914</v>
       </c>
@@ -4056,19 +4119,23 @@
         <v>8</v>
       </c>
       <c r="J16" s="5">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="K16" s="5">
         <v>321</v>
       </c>
-      <c r="K16" s="5">
+      <c r="L16" s="5">
         <v>66</v>
       </c>
-      <c r="L16" s="5">
+      <c r="M16" s="5">
         <v>46</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="6">
         <v>43915</v>
       </c>
@@ -4096,20 +4163,23 @@
       <c r="I17" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J17" s="5">
+      <c r="J17" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K17" s="5">
         <v>375</v>
       </c>
-      <c r="K17" s="5">
+      <c r="L17" s="5">
         <v>79</v>
       </c>
-      <c r="L17" s="5">
+      <c r="M17" s="5">
         <v>46</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="6">
         <v>43916</v>
       </c>
@@ -4137,20 +4207,23 @@
       <c r="I18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J18" s="5">
+      <c r="J18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K18" s="5">
         <v>445</v>
       </c>
-      <c r="K18" s="5">
+      <c r="L18" s="5">
         <v>91</v>
       </c>
-      <c r="L18" s="5">
+      <c r="M18" s="5">
         <v>46</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="6">
         <v>43917</v>
       </c>
@@ -4179,19 +4252,23 @@
         <v>8</v>
       </c>
       <c r="J19" s="5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K19" s="5">
         <v>506</v>
       </c>
-      <c r="K19" s="5">
+      <c r="L19" s="5">
         <v>103</v>
       </c>
-      <c r="L19" s="5">
+      <c r="M19" s="5">
         <v>47</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="6">
         <v>43918</v>
       </c>
@@ -4220,19 +4297,23 @@
         <v>8</v>
       </c>
       <c r="J20" s="5">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="K20" s="5">
         <v>578</v>
       </c>
-      <c r="K20" s="5">
+      <c r="L20" s="5">
         <v>111</v>
       </c>
-      <c r="L20" s="5">
+      <c r="M20" s="5">
         <v>47</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="21" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="6">
         <v>43919</v>
       </c>
@@ -4242,8 +4323,8 @@
       <c r="C21" s="5">
         <v>2677</v>
       </c>
-      <c r="D21" s="5" t="s">
-        <v>8</v>
+      <c r="D21" s="5">
+        <v>2615</v>
       </c>
       <c r="E21" s="5">
         <v>202</v>
@@ -4261,19 +4342,23 @@
         <v>8</v>
       </c>
       <c r="J21" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K21" s="5">
         <v>674</v>
       </c>
-      <c r="K21" s="5">
+      <c r="L21" s="5">
         <v>118</v>
       </c>
-      <c r="L21" s="5">
+      <c r="M21" s="5">
         <v>47</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="6">
         <v>43920</v>
       </c>
@@ -4283,8 +4368,8 @@
       <c r="C22" s="5">
         <v>2990</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>8</v>
+      <c r="D22" s="5">
+        <v>2910</v>
       </c>
       <c r="E22" s="5">
         <v>313</v>
@@ -4302,19 +4387,23 @@
         <v>8</v>
       </c>
       <c r="J22" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K22" s="5">
         <v>752</v>
       </c>
-      <c r="K22" s="5">
+      <c r="L22" s="5">
         <v>134</v>
       </c>
-      <c r="L22" s="5">
+      <c r="M22" s="5">
         <v>48</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A23" s="6">
         <v>43921</v>
       </c>
@@ -4324,8 +4413,8 @@
       <c r="C23" s="5">
         <v>3282</v>
       </c>
-      <c r="D23" s="5" t="s">
-        <v>8</v>
+      <c r="D23" s="5">
+        <v>3235</v>
       </c>
       <c r="E23" s="5">
         <v>292</v>
@@ -4339,23 +4428,27 @@
       <c r="H23" s="5">
         <v>91</v>
       </c>
-      <c r="I23" s="5" t="s">
-        <v>8</v>
+      <c r="I23" s="5">
+        <v>71</v>
       </c>
       <c r="J23" s="5">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="K23" s="5">
         <v>841</v>
       </c>
-      <c r="K23" s="5">
+      <c r="L23" s="5">
         <v>160</v>
       </c>
-      <c r="L23" s="5">
+      <c r="M23" s="5">
         <v>48</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A24" s="6">
         <v>43922</v>
       </c>
@@ -4365,8 +4458,8 @@
       <c r="C24" s="5">
         <v>3655</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>8</v>
+      <c r="D24" s="5">
+        <v>3447</v>
       </c>
       <c r="E24" s="5">
         <v>373</v>
@@ -4380,23 +4473,27 @@
       <c r="H24" s="5">
         <v>113</v>
       </c>
-      <c r="I24" s="5" t="s">
-        <v>8</v>
+      <c r="I24" s="5">
+        <v>85</v>
       </c>
       <c r="J24" s="5">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="K24" s="5">
         <v>948</v>
       </c>
-      <c r="K24" s="5">
+      <c r="L24" s="5">
         <v>171</v>
       </c>
-      <c r="L24" s="5">
+      <c r="M24" s="5">
         <v>48</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A25" s="6">
         <v>43923</v>
       </c>
@@ -4406,8 +4503,8 @@
       <c r="C25" s="5">
         <v>4014</v>
       </c>
-      <c r="D25" s="5" t="s">
-        <v>8</v>
+      <c r="D25" s="5">
+        <v>3849</v>
       </c>
       <c r="E25" s="5">
         <v>359</v>
@@ -4421,23 +4518,27 @@
       <c r="H25" s="5">
         <v>131</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>8</v>
+      <c r="I25" s="5">
+        <v>98</v>
       </c>
       <c r="J25" s="5">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="K25" s="5">
         <v>1084</v>
       </c>
-      <c r="K25" s="5">
+      <c r="L25" s="5">
         <v>206</v>
       </c>
-      <c r="L25" s="5">
+      <c r="M25" s="5">
         <v>48</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="6">
         <v>43924</v>
       </c>
@@ -4447,8 +4548,8 @@
       <c r="C26" s="5">
         <v>4443</v>
       </c>
-      <c r="D26" s="5" t="s">
-        <v>8</v>
+      <c r="D26" s="5">
+        <v>4273</v>
       </c>
       <c r="E26" s="5">
         <v>429</v>
@@ -4462,23 +4563,27 @@
       <c r="H26" s="5">
         <v>151</v>
       </c>
-      <c r="I26" s="5" t="s">
-        <v>8</v>
+      <c r="I26" s="5">
+        <v>120</v>
       </c>
       <c r="J26" s="5">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K26" s="5">
         <v>1163</v>
       </c>
-      <c r="K26" s="5">
+      <c r="L26" s="5">
         <v>236</v>
       </c>
-      <c r="L26" s="5">
+      <c r="M26" s="5">
         <v>48</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A27" s="6">
         <v>43925</v>
       </c>
@@ -4488,11 +4593,11 @@
       <c r="C27" s="5">
         <v>4916</v>
       </c>
-      <c r="D27" s="5" t="s">
-        <v>8</v>
+      <c r="D27" s="5">
+        <v>4604</v>
       </c>
       <c r="E27" s="5">
-        <f t="shared" ref="E27:E47" si="0">C27-C26</f>
+        <f t="shared" ref="E27:E47" si="1">C27-C26</f>
         <v>473</v>
       </c>
       <c r="F27" s="5">
@@ -4504,23 +4609,27 @@
       <c r="H27" s="5">
         <v>167</v>
       </c>
-      <c r="I27" s="5" t="s">
-        <v>8</v>
+      <c r="I27" s="5">
+        <v>137</v>
       </c>
       <c r="J27" s="5">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K27" s="5">
         <v>1263</v>
       </c>
-      <c r="K27" s="5">
+      <c r="L27" s="5">
         <v>260</v>
       </c>
-      <c r="L27" s="5">
+      <c r="M27" s="5">
         <v>49</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="28" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A28" s="6">
         <v>43926</v>
       </c>
@@ -4530,11 +4639,11 @@
       <c r="C28" s="5">
         <v>5593</v>
       </c>
-      <c r="D28" s="5" t="s">
-        <v>8</v>
+      <c r="D28" s="5">
+        <v>4994</v>
       </c>
       <c r="E28" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>677</v>
       </c>
       <c r="F28" s="5">
@@ -4546,23 +4655,27 @@
       <c r="H28" s="5">
         <v>204</v>
       </c>
-      <c r="I28" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J28">
+      <c r="I28" s="5">
+        <v>158</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="K28">
         <v>1388</v>
       </c>
-      <c r="K28" s="5">
+      <c r="L28" s="5">
         <v>270</v>
       </c>
-      <c r="L28" s="5">
+      <c r="M28" s="5">
         <v>48</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="29" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>43927</v>
       </c>
@@ -4572,11 +4685,11 @@
       <c r="C29" s="5">
         <v>5981</v>
       </c>
-      <c r="D29" s="5" t="s">
-        <v>8</v>
+      <c r="D29" s="5">
+        <v>5364</v>
       </c>
       <c r="E29" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>388</v>
       </c>
       <c r="F29" s="5">
@@ -4588,23 +4701,27 @@
       <c r="H29" s="5">
         <v>223</v>
       </c>
-      <c r="I29" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J29">
+      <c r="I29" s="5">
+        <v>174</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="K29">
         <v>1568</v>
       </c>
-      <c r="K29" s="5">
+      <c r="L29" s="5">
         <v>299</v>
       </c>
-      <c r="L29" s="5">
+      <c r="M29" s="5">
         <v>48</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="30" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>43928</v>
       </c>
@@ -4614,11 +4731,11 @@
       <c r="C30" s="5">
         <v>6444</v>
       </c>
-      <c r="D30" s="5" t="s">
-        <v>8</v>
+      <c r="D30" s="5">
+        <v>5709</v>
       </c>
       <c r="E30" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>463</v>
       </c>
       <c r="F30" s="5">
@@ -4630,23 +4747,27 @@
       <c r="H30" s="5">
         <v>257</v>
       </c>
-      <c r="I30" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J30">
+      <c r="I30" s="5">
+        <v>210</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="K30">
         <v>1765</v>
       </c>
-      <c r="K30" s="5">
+      <c r="L30" s="5">
         <v>317</v>
       </c>
-      <c r="L30" s="5">
+      <c r="M30" s="5">
         <v>48</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>43929</v>
       </c>
@@ -4656,11 +4777,11 @@
       <c r="C31" s="5">
         <v>7071</v>
       </c>
-      <c r="D31" s="5" t="s">
-        <v>8</v>
+      <c r="D31" s="5">
+        <v>6074</v>
       </c>
       <c r="E31" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>627</v>
       </c>
       <c r="F31">
@@ -4672,23 +4793,27 @@
       <c r="H31" s="5">
         <v>283</v>
       </c>
-      <c r="I31" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J31">
+      <c r="I31" s="5">
+        <v>235</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="K31">
         <v>1949</v>
       </c>
-      <c r="K31">
+      <c r="L31">
         <v>333</v>
       </c>
-      <c r="L31">
+      <c r="M31">
         <v>48</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>43930</v>
       </c>
@@ -4698,11 +4823,11 @@
       <c r="C32">
         <v>7787</v>
       </c>
-      <c r="D32" s="5" t="s">
-        <v>8</v>
+      <c r="D32" s="5">
+        <v>6574</v>
       </c>
       <c r="E32" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>716</v>
       </c>
       <c r="F32">
@@ -4714,23 +4839,27 @@
       <c r="H32" s="5">
         <v>314</v>
       </c>
-      <c r="I32" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J32">
+      <c r="I32" s="5">
+        <v>263</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="K32">
         <v>2141</v>
       </c>
-      <c r="K32">
+      <c r="L32">
         <v>356</v>
       </c>
-      <c r="L32">
+      <c r="M32">
         <v>48</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="33" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>43931</v>
       </c>
@@ -4740,11 +4869,11 @@
       <c r="C33" s="5">
         <v>8496</v>
       </c>
-      <c r="D33" s="5" t="s">
-        <v>8</v>
+      <c r="D33" s="5">
+        <v>7054</v>
       </c>
       <c r="E33" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>709</v>
       </c>
       <c r="F33">
@@ -4756,23 +4885,27 @@
       <c r="H33" s="5">
         <v>329</v>
       </c>
-      <c r="I33" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J33">
+      <c r="I33" s="5">
+        <v>287</v>
+      </c>
+      <c r="J33" s="5">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K33">
         <v>2312</v>
       </c>
-      <c r="K33">
+      <c r="L33">
         <v>383</v>
       </c>
-      <c r="L33">
+      <c r="M33">
         <v>48</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="34" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>43932</v>
       </c>
@@ -4786,7 +4919,7 @@
         <v>8</v>
       </c>
       <c r="E34" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>988</v>
       </c>
       <c r="F34">
@@ -4798,23 +4931,27 @@
       <c r="H34" s="5">
         <v>362</v>
       </c>
-      <c r="I34" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J34">
+      <c r="I34" s="5">
+        <v>320</v>
+      </c>
+      <c r="J34" s="5">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K34">
         <v>2489</v>
       </c>
-      <c r="K34">
+      <c r="L34">
         <v>401</v>
       </c>
-      <c r="L34">
+      <c r="M34">
         <v>48</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>43933</v>
       </c>
@@ -4824,11 +4961,11 @@
       <c r="C35" s="5">
         <v>10385</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>8</v>
+      <c r="D35" s="5">
+        <v>9655</v>
       </c>
       <c r="E35" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>901</v>
       </c>
       <c r="F35">
@@ -4840,23 +4977,27 @@
       <c r="H35" s="5">
         <v>395</v>
       </c>
-      <c r="I35" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J35">
+      <c r="I35" s="5">
+        <v>334</v>
+      </c>
+      <c r="J35" s="5">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="K35">
         <v>2707</v>
       </c>
-      <c r="K35">
+      <c r="L35">
         <v>408</v>
       </c>
-      <c r="L35">
+      <c r="M35">
         <v>48</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="36" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>43934</v>
       </c>
@@ -4866,11 +5007,11 @@
       <c r="C36" s="5">
         <v>11261</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>8</v>
+      <c r="D36" s="5">
+        <v>10647</v>
       </c>
       <c r="E36" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>876</v>
       </c>
       <c r="F36">
@@ -4882,23 +5023,27 @@
       <c r="H36" s="5">
         <v>435</v>
       </c>
-      <c r="I36" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J36">
+      <c r="I36" s="5">
+        <v>365</v>
+      </c>
+      <c r="J36" s="5">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="K36">
         <v>2872</v>
       </c>
-      <c r="K36">
+      <c r="L36">
         <v>413</v>
       </c>
-      <c r="L36">
+      <c r="M36">
         <v>48</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="37" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>43935</v>
       </c>
@@ -4908,11 +5053,11 @@
       <c r="C37" s="5">
         <v>12425</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>8</v>
+      <c r="D37" s="5">
+        <v>11479</v>
       </c>
       <c r="E37" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1164</v>
       </c>
       <c r="F37">
@@ -4924,23 +5069,27 @@
       <c r="H37" s="5">
         <v>480</v>
       </c>
-      <c r="I37" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J37">
+      <c r="I37" s="5">
+        <v>406</v>
+      </c>
+      <c r="J37" s="5">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K37">
         <v>2451</v>
       </c>
-      <c r="K37">
+      <c r="L37">
         <v>425</v>
       </c>
-      <c r="L37">
+      <c r="M37">
         <v>48</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="38" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>43936</v>
       </c>
@@ -4950,11 +5099,11 @@
       <c r="C38" s="5">
         <v>13012</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>8</v>
+      <c r="D38" s="5">
+        <v>12547</v>
       </c>
       <c r="E38" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>587</v>
       </c>
       <c r="F38">
@@ -4966,23 +5115,27 @@
       <c r="H38" s="5">
         <v>521</v>
       </c>
-      <c r="I38" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J38">
+      <c r="I38" s="5">
+        <v>444</v>
+      </c>
+      <c r="J38" s="5">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="K38">
         <v>2723</v>
       </c>
-      <c r="K38">
+      <c r="L38">
         <v>436</v>
       </c>
-      <c r="L38">
+      <c r="M38">
         <v>48</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="39" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>43937</v>
       </c>
@@ -4992,11 +5145,11 @@
       <c r="C39" s="5">
         <v>13746</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>8</v>
+      <c r="D39" s="5">
+        <v>13271</v>
       </c>
       <c r="E39" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>734</v>
       </c>
       <c r="F39">
@@ -5008,23 +5161,27 @@
       <c r="H39" s="5">
         <v>566</v>
       </c>
-      <c r="I39" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J39">
+      <c r="I39" s="5">
+        <v>486</v>
+      </c>
+      <c r="J39" s="5">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="K39">
         <v>3573</v>
       </c>
-      <c r="K39">
+      <c r="L39">
         <v>454</v>
       </c>
-      <c r="L39">
+      <c r="M39">
         <v>48</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="40" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>43938</v>
       </c>
@@ -5034,11 +5191,11 @@
       <c r="C40" s="5">
         <v>14602</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>8</v>
+      <c r="D40" s="5">
+        <v>13980</v>
       </c>
       <c r="E40" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>856</v>
       </c>
       <c r="F40">
@@ -5050,23 +5207,27 @@
       <c r="H40" s="5">
         <v>605</v>
       </c>
-      <c r="I40" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J40">
+      <c r="I40" s="5">
+        <v>530</v>
+      </c>
+      <c r="J40" s="5">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="K40">
         <v>3788</v>
       </c>
-      <c r="K40">
+      <c r="L40">
         <v>472</v>
       </c>
-      <c r="L40">
+      <c r="M40">
         <v>48</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="41" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>43939</v>
       </c>
@@ -5076,11 +5237,11 @@
       <c r="C41" s="5">
         <v>15185</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>8</v>
+      <c r="D41" s="5">
+        <v>14758</v>
       </c>
       <c r="E41" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>583</v>
       </c>
       <c r="F41">
@@ -5092,23 +5253,27 @@
       <c r="H41" s="5">
         <v>642</v>
       </c>
-      <c r="I41" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J41">
+      <c r="I41" s="5">
+        <v>571</v>
+      </c>
+      <c r="J41" s="5">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="K41">
         <v>4009</v>
       </c>
-      <c r="K41">
+      <c r="L41">
         <v>478</v>
       </c>
-      <c r="L41">
+      <c r="M41">
         <v>48</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="42" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>43940</v>
       </c>
@@ -5118,11 +5283,11 @@
       <c r="C42" s="5">
         <v>15464</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>8</v>
+      <c r="D42" s="5">
+        <v>15251</v>
       </c>
       <c r="E42" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>279</v>
       </c>
       <c r="F42">
@@ -5134,23 +5299,27 @@
       <c r="H42" s="5">
         <v>719</v>
       </c>
-      <c r="I42" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J42">
+      <c r="I42" s="5">
+        <v>610</v>
+      </c>
+      <c r="J42" s="5">
+        <f t="shared" si="0"/>
+        <v>77</v>
+      </c>
+      <c r="K42">
         <v>4180</v>
       </c>
-      <c r="K42">
+      <c r="L42">
         <v>491</v>
       </c>
-      <c r="L42">
+      <c r="M42">
         <v>48</v>
       </c>
-      <c r="M42" t="s">
+      <c r="N42" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="43" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>43941</v>
       </c>
@@ -5160,11 +5329,11 @@
       <c r="C43" s="5">
         <v>15871</v>
       </c>
-      <c r="D43" s="5" t="s">
-        <v>8</v>
+      <c r="D43" s="5">
+        <v>15652</v>
       </c>
       <c r="E43" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>407</v>
       </c>
       <c r="F43">
@@ -5176,23 +5345,27 @@
       <c r="H43" s="5">
         <v>757</v>
       </c>
-      <c r="I43" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J43">
+      <c r="I43" s="5">
+        <v>687</v>
+      </c>
+      <c r="J43" s="5">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="K43">
         <v>4393</v>
       </c>
-      <c r="K43">
+      <c r="L43">
         <v>507</v>
       </c>
-      <c r="L43">
+      <c r="M43">
         <v>48</v>
       </c>
-      <c r="M43" t="s">
+      <c r="N43" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="44" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>43942</v>
       </c>
@@ -5206,7 +5379,7 @@
         <v>16040</v>
       </c>
       <c r="E44" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>568</v>
       </c>
       <c r="F44">
@@ -5221,20 +5394,24 @@
       <c r="I44" s="5">
         <v>730</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="K44">
         <v>4545</v>
       </c>
-      <c r="K44">
+      <c r="L44">
         <v>522</v>
       </c>
-      <c r="L44">
+      <c r="M44">
         <v>48</v>
       </c>
-      <c r="M44" t="s">
+      <c r="N44" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="45" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43943</v>
       </c>
@@ -5248,7 +5425,7 @@
         <v>16671</v>
       </c>
       <c r="E45" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>981</v>
       </c>
       <c r="F45">
@@ -5263,20 +5440,24 @@
       <c r="I45" s="5">
         <v>769</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="5">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="K45">
         <v>4713</v>
       </c>
-      <c r="K45">
+      <c r="L45">
         <v>548</v>
       </c>
-      <c r="L45">
+      <c r="M45">
         <v>48</v>
       </c>
-      <c r="M45" t="s">
+      <c r="N45" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="46" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>43944</v>
       </c>
@@ -5290,7 +5471,7 @@
         <v>8</v>
       </c>
       <c r="E46" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>187</v>
       </c>
       <c r="F46" t="s">
@@ -5305,8 +5486,9 @@
       <c r="I46" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J46" t="s">
-        <v>8</v>
+      <c r="J46" s="5">
+        <f t="shared" si="0"/>
+        <v>-27</v>
       </c>
       <c r="K46" t="s">
         <v>8</v>
@@ -5315,10 +5497,13 @@
         <v>8</v>
       </c>
       <c r="M46" t="s">
+        <v>8</v>
+      </c>
+      <c r="N46" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="47" spans="1:13" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>43945</v>
       </c>
@@ -5332,7 +5517,7 @@
         <v>8</v>
       </c>
       <c r="E47" s="5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>577</v>
       </c>
       <c r="F47" t="s">
@@ -5347,8 +5532,9 @@
       <c r="I47" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J47" t="s">
-        <v>8</v>
+      <c r="J47" s="5">
+        <f>H47-H46</f>
+        <v>35</v>
       </c>
       <c r="K47" t="s">
         <v>8</v>
@@ -5357,6 +5543,9 @@
         <v>8</v>
       </c>
       <c r="M47" t="s">
+        <v>8</v>
+      </c>
+      <c r="N47" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added Irish adjacency matrix
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE45F31B-EDD0-A941-B468-1D48505F4D95}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F6AF4-7138-E240-964B-18D3ABF4D68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,8 @@
     <sheet name="NI_gender" sheetId="8" r:id="rId10"/>
     <sheet name="NI_age" sheetId="9" r:id="rId11"/>
     <sheet name="NI_district" sheetId="10" r:id="rId12"/>
-    <sheet name="NI_county_lookup" sheetId="11" r:id="rId13"/>
+    <sheet name="Adjacency_matrix" sheetId="14" r:id="rId13"/>
+    <sheet name="NI_county_lookup" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3966" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4018" uniqueCount="222">
   <si>
     <t>Date</t>
   </si>
@@ -1671,7 +1672,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C5E2DA3-023C-FF46-A014-0C2E672468A0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -6716,6 +6717,2262 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349ABED6-B9F8-C047-A7E7-BF15BC014788}">
+  <dimension ref="A1:AA27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>36</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O1" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>28</v>
+      </c>
+      <c r="U1" t="s">
+        <v>29</v>
+      </c>
+      <c r="V1" t="s">
+        <v>30</v>
+      </c>
+      <c r="W1" t="s">
+        <v>31</v>
+      </c>
+      <c r="X1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>33</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2">
+        <v>1</v>
+      </c>
+      <c r="L2">
+        <v>1</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>1</v>
+      </c>
+      <c r="AA2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>1</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>0</v>
+      </c>
+      <c r="R3">
+        <v>1</v>
+      </c>
+      <c r="S3">
+        <v>1</v>
+      </c>
+      <c r="T3">
+        <v>0</v>
+      </c>
+      <c r="U3">
+        <v>0</v>
+      </c>
+      <c r="V3">
+        <v>0</v>
+      </c>
+      <c r="W3">
+        <v>0</v>
+      </c>
+      <c r="X3">
+        <v>0</v>
+      </c>
+      <c r="Y3">
+        <v>1</v>
+      </c>
+      <c r="Z3">
+        <v>0</v>
+      </c>
+      <c r="AA3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+      <c r="N4">
+        <v>1</v>
+      </c>
+      <c r="O4">
+        <v>0</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+      <c r="Q4">
+        <v>0</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4">
+        <v>0</v>
+      </c>
+      <c r="T4">
+        <v>0</v>
+      </c>
+      <c r="U4">
+        <v>0</v>
+      </c>
+      <c r="V4">
+        <v>0</v>
+      </c>
+      <c r="W4">
+        <v>1</v>
+      </c>
+      <c r="X4">
+        <v>0</v>
+      </c>
+      <c r="Y4">
+        <v>0</v>
+      </c>
+      <c r="Z4">
+        <v>0</v>
+      </c>
+      <c r="AA4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+      <c r="N5">
+        <v>1</v>
+      </c>
+      <c r="O5">
+        <v>0</v>
+      </c>
+      <c r="P5">
+        <v>0</v>
+      </c>
+      <c r="Q5">
+        <v>0</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5">
+        <v>0</v>
+      </c>
+      <c r="T5">
+        <v>0</v>
+      </c>
+      <c r="U5">
+        <v>0</v>
+      </c>
+      <c r="V5">
+        <v>0</v>
+      </c>
+      <c r="W5">
+        <v>1</v>
+      </c>
+      <c r="X5">
+        <v>1</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>0</v>
+      </c>
+      <c r="L6">
+        <v>0</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>0</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+      <c r="P6">
+        <v>0</v>
+      </c>
+      <c r="Q6">
+        <v>0</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6">
+        <v>0</v>
+      </c>
+      <c r="T6">
+        <v>0</v>
+      </c>
+      <c r="U6">
+        <v>0</v>
+      </c>
+      <c r="V6">
+        <v>0</v>
+      </c>
+      <c r="W6">
+        <v>0</v>
+      </c>
+      <c r="X6">
+        <v>0</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7">
+        <v>0</v>
+      </c>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>1</v>
+      </c>
+      <c r="K7">
+        <v>0</v>
+      </c>
+      <c r="L7">
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+      <c r="Q7">
+        <v>0</v>
+      </c>
+      <c r="R7">
+        <v>1</v>
+      </c>
+      <c r="S7">
+        <v>0</v>
+      </c>
+      <c r="T7">
+        <v>0</v>
+      </c>
+      <c r="U7">
+        <v>0</v>
+      </c>
+      <c r="V7">
+        <v>0</v>
+      </c>
+      <c r="W7">
+        <v>0</v>
+      </c>
+      <c r="X7">
+        <v>0</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <v>0</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
+      <c r="L8">
+        <v>0</v>
+      </c>
+      <c r="M8">
+        <v>0</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>0</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+      <c r="Q8">
+        <v>1</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8">
+        <v>0</v>
+      </c>
+      <c r="T8">
+        <v>1</v>
+      </c>
+      <c r="U8">
+        <v>1</v>
+      </c>
+      <c r="V8">
+        <v>0</v>
+      </c>
+      <c r="W8">
+        <v>1</v>
+      </c>
+      <c r="X8">
+        <v>0</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9">
+        <v>0</v>
+      </c>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <v>0</v>
+      </c>
+      <c r="L9">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <v>0</v>
+      </c>
+      <c r="Q9">
+        <v>0</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9">
+        <v>0</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9">
+        <v>0</v>
+      </c>
+      <c r="V9">
+        <v>0</v>
+      </c>
+      <c r="W9">
+        <v>0</v>
+      </c>
+      <c r="X9">
+        <v>0</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <v>0</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <v>0</v>
+      </c>
+      <c r="L10">
+        <v>1</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+      <c r="Q10">
+        <v>0</v>
+      </c>
+      <c r="R10">
+        <v>1</v>
+      </c>
+      <c r="S10">
+        <v>0</v>
+      </c>
+      <c r="T10">
+        <v>1</v>
+      </c>
+      <c r="U10">
+        <v>0</v>
+      </c>
+      <c r="V10">
+        <v>0</v>
+      </c>
+      <c r="W10">
+        <v>0</v>
+      </c>
+      <c r="X10">
+        <v>0</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11">
+        <v>0</v>
+      </c>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>0</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <v>0</v>
+      </c>
+      <c r="L11">
+        <v>1</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <v>0</v>
+      </c>
+      <c r="Q11">
+        <v>0</v>
+      </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
+      <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11">
+        <v>0</v>
+      </c>
+      <c r="V11">
+        <v>0</v>
+      </c>
+      <c r="W11">
+        <v>1</v>
+      </c>
+      <c r="X11">
+        <v>1</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11">
+        <v>1</v>
+      </c>
+      <c r="AA11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>1</v>
+      </c>
+      <c r="K12">
+        <v>1</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <v>0</v>
+      </c>
+      <c r="Q12">
+        <v>0</v>
+      </c>
+      <c r="R12">
+        <v>0</v>
+      </c>
+      <c r="S12">
+        <v>0</v>
+      </c>
+      <c r="T12">
+        <v>1</v>
+      </c>
+      <c r="U12">
+        <v>0</v>
+      </c>
+      <c r="V12">
+        <v>0</v>
+      </c>
+      <c r="W12">
+        <v>1</v>
+      </c>
+      <c r="X12">
+        <v>0</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>1</v>
+      </c>
+      <c r="P13">
+        <v>0</v>
+      </c>
+      <c r="Q13">
+        <v>0</v>
+      </c>
+      <c r="R13">
+        <v>0</v>
+      </c>
+      <c r="S13">
+        <v>0</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13">
+        <v>1</v>
+      </c>
+      <c r="V13">
+        <v>1</v>
+      </c>
+      <c r="W13">
+        <v>0</v>
+      </c>
+      <c r="X13">
+        <v>0</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>23</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0</v>
+      </c>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <v>0</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>0</v>
+      </c>
+      <c r="P14">
+        <v>0</v>
+      </c>
+      <c r="Q14">
+        <v>0</v>
+      </c>
+      <c r="R14">
+        <v>0</v>
+      </c>
+      <c r="S14">
+        <v>0</v>
+      </c>
+      <c r="T14">
+        <v>0</v>
+      </c>
+      <c r="U14">
+        <v>0</v>
+      </c>
+      <c r="V14">
+        <v>0</v>
+      </c>
+      <c r="W14">
+        <v>1</v>
+      </c>
+      <c r="X14">
+        <v>0</v>
+      </c>
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>24</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+      <c r="G15">
+        <v>0</v>
+      </c>
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="I15">
+        <v>0</v>
+      </c>
+      <c r="J15">
+        <v>0</v>
+      </c>
+      <c r="K15">
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>0</v>
+      </c>
+      <c r="P15">
+        <v>0</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
+        <v>0</v>
+      </c>
+      <c r="S15">
+        <v>0</v>
+      </c>
+      <c r="T15">
+        <v>0</v>
+      </c>
+      <c r="U15">
+        <v>1</v>
+      </c>
+      <c r="V15">
+        <v>0</v>
+      </c>
+      <c r="W15">
+        <v>0</v>
+      </c>
+      <c r="X15">
+        <v>0</v>
+      </c>
+      <c r="Y15">
+        <v>1</v>
+      </c>
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16">
+        <v>0</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="I16">
+        <v>0</v>
+      </c>
+      <c r="J16">
+        <v>0</v>
+      </c>
+      <c r="K16">
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+      <c r="P16">
+        <v>0</v>
+      </c>
+      <c r="Q16">
+        <v>0</v>
+      </c>
+      <c r="R16">
+        <v>1</v>
+      </c>
+      <c r="S16">
+        <v>1</v>
+      </c>
+      <c r="T16">
+        <v>0</v>
+      </c>
+      <c r="U16">
+        <v>0</v>
+      </c>
+      <c r="V16">
+        <v>0</v>
+      </c>
+      <c r="W16">
+        <v>0</v>
+      </c>
+      <c r="X16">
+        <v>0</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <v>0</v>
+      </c>
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <v>0</v>
+      </c>
+      <c r="M17">
+        <v>0</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+      <c r="P17">
+        <v>0</v>
+      </c>
+      <c r="Q17">
+        <v>0</v>
+      </c>
+      <c r="R17">
+        <v>0</v>
+      </c>
+      <c r="S17">
+        <v>0</v>
+      </c>
+      <c r="T17">
+        <v>0</v>
+      </c>
+      <c r="U17">
+        <v>1</v>
+      </c>
+      <c r="V17">
+        <v>1</v>
+      </c>
+      <c r="W17">
+        <v>0</v>
+      </c>
+      <c r="X17">
+        <v>0</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>27</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="I18">
+        <v>0</v>
+      </c>
+      <c r="J18">
+        <v>1</v>
+      </c>
+      <c r="K18">
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <v>0</v>
+      </c>
+      <c r="M18">
+        <v>0</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>0</v>
+      </c>
+      <c r="P18">
+        <v>1</v>
+      </c>
+      <c r="Q18">
+        <v>0</v>
+      </c>
+      <c r="R18">
+        <v>0</v>
+      </c>
+      <c r="S18">
+        <v>1</v>
+      </c>
+      <c r="T18">
+        <v>1</v>
+      </c>
+      <c r="U18">
+        <v>0</v>
+      </c>
+      <c r="V18">
+        <v>0</v>
+      </c>
+      <c r="W18">
+        <v>0</v>
+      </c>
+      <c r="X18">
+        <v>0</v>
+      </c>
+      <c r="Y18">
+        <v>1</v>
+      </c>
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="I19">
+        <v>0</v>
+      </c>
+      <c r="J19">
+        <v>0</v>
+      </c>
+      <c r="K19">
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <v>0</v>
+      </c>
+      <c r="M19">
+        <v>0</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>0</v>
+      </c>
+      <c r="P19">
+        <v>1</v>
+      </c>
+      <c r="Q19">
+        <v>0</v>
+      </c>
+      <c r="R19">
+        <v>1</v>
+      </c>
+      <c r="S19">
+        <v>0</v>
+      </c>
+      <c r="T19">
+        <v>0</v>
+      </c>
+      <c r="U19">
+        <v>0</v>
+      </c>
+      <c r="V19">
+        <v>0</v>
+      </c>
+      <c r="W19">
+        <v>0</v>
+      </c>
+      <c r="X19">
+        <v>0</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>1</v>
+      </c>
+      <c r="I20">
+        <v>0</v>
+      </c>
+      <c r="J20">
+        <v>1</v>
+      </c>
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>1</v>
+      </c>
+      <c r="M20">
+        <v>0</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>0</v>
+      </c>
+      <c r="P20">
+        <v>0</v>
+      </c>
+      <c r="Q20">
+        <v>0</v>
+      </c>
+      <c r="R20">
+        <v>1</v>
+      </c>
+      <c r="S20">
+        <v>0</v>
+      </c>
+      <c r="T20">
+        <v>0</v>
+      </c>
+      <c r="U20">
+        <v>1</v>
+      </c>
+      <c r="V20">
+        <v>0</v>
+      </c>
+      <c r="W20">
+        <v>1</v>
+      </c>
+      <c r="X20">
+        <v>0</v>
+      </c>
+      <c r="Y20">
+        <v>1</v>
+      </c>
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>1</v>
+      </c>
+      <c r="I21">
+        <v>0</v>
+      </c>
+      <c r="J21">
+        <v>0</v>
+      </c>
+      <c r="K21">
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <v>0</v>
+      </c>
+      <c r="M21">
+        <v>1</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+      <c r="P21">
+        <v>0</v>
+      </c>
+      <c r="Q21">
+        <v>1</v>
+      </c>
+      <c r="R21">
+        <v>0</v>
+      </c>
+      <c r="S21">
+        <v>0</v>
+      </c>
+      <c r="T21">
+        <v>1</v>
+      </c>
+      <c r="U21">
+        <v>0</v>
+      </c>
+      <c r="V21">
+        <v>1</v>
+      </c>
+      <c r="W21">
+        <v>0</v>
+      </c>
+      <c r="X21">
+        <v>0</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0</v>
+      </c>
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>0</v>
+      </c>
+      <c r="I22">
+        <v>0</v>
+      </c>
+      <c r="J22">
+        <v>0</v>
+      </c>
+      <c r="K22">
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <v>0</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+      <c r="P22">
+        <v>0</v>
+      </c>
+      <c r="Q22">
+        <v>1</v>
+      </c>
+      <c r="R22">
+        <v>0</v>
+      </c>
+      <c r="S22">
+        <v>0</v>
+      </c>
+      <c r="T22">
+        <v>0</v>
+      </c>
+      <c r="U22">
+        <v>1</v>
+      </c>
+      <c r="V22">
+        <v>0</v>
+      </c>
+      <c r="W22">
+        <v>0</v>
+      </c>
+      <c r="X22">
+        <v>0</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>31</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+      <c r="C23">
+        <v>0</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>0</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23">
+        <v>1</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23">
+        <v>0</v>
+      </c>
+      <c r="K23">
+        <v>1</v>
+      </c>
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>1</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+      <c r="P23">
+        <v>0</v>
+      </c>
+      <c r="Q23">
+        <v>0</v>
+      </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
+      <c r="S23">
+        <v>0</v>
+      </c>
+      <c r="T23">
+        <v>1</v>
+      </c>
+      <c r="U23">
+        <v>0</v>
+      </c>
+      <c r="V23">
+        <v>0</v>
+      </c>
+      <c r="W23">
+        <v>0</v>
+      </c>
+      <c r="X23">
+        <v>1</v>
+      </c>
+      <c r="Y23">
+        <v>0</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="E24">
+        <v>1</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24">
+        <v>0</v>
+      </c>
+      <c r="K24">
+        <v>1</v>
+      </c>
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+      <c r="P24">
+        <v>0</v>
+      </c>
+      <c r="Q24">
+        <v>0</v>
+      </c>
+      <c r="R24">
+        <v>0</v>
+      </c>
+      <c r="S24">
+        <v>0</v>
+      </c>
+      <c r="T24">
+        <v>0</v>
+      </c>
+      <c r="U24">
+        <v>0</v>
+      </c>
+      <c r="V24">
+        <v>0</v>
+      </c>
+      <c r="W24">
+        <v>1</v>
+      </c>
+      <c r="X24">
+        <v>0</v>
+      </c>
+      <c r="Y24">
+        <v>0</v>
+      </c>
+      <c r="Z24">
+        <v>1</v>
+      </c>
+      <c r="AA24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>33</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>0</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25">
+        <v>0</v>
+      </c>
+      <c r="I25">
+        <v>0</v>
+      </c>
+      <c r="J25">
+        <v>0</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <v>0</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+      <c r="P25">
+        <v>0</v>
+      </c>
+      <c r="Q25">
+        <v>0</v>
+      </c>
+      <c r="R25">
+        <v>1</v>
+      </c>
+      <c r="S25">
+        <v>0</v>
+      </c>
+      <c r="T25">
+        <v>1</v>
+      </c>
+      <c r="U25">
+        <v>0</v>
+      </c>
+      <c r="V25">
+        <v>0</v>
+      </c>
+      <c r="W25">
+        <v>0</v>
+      </c>
+      <c r="X25">
+        <v>0</v>
+      </c>
+      <c r="Y25">
+        <v>0</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>34</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0</v>
+      </c>
+      <c r="G26">
+        <v>0</v>
+      </c>
+      <c r="H26">
+        <v>0</v>
+      </c>
+      <c r="I26">
+        <v>0</v>
+      </c>
+      <c r="J26">
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>1</v>
+      </c>
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="Q26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>0</v>
+      </c>
+      <c r="U26">
+        <v>0</v>
+      </c>
+      <c r="V26">
+        <v>0</v>
+      </c>
+      <c r="W26">
+        <v>0</v>
+      </c>
+      <c r="X26">
+        <v>1</v>
+      </c>
+      <c r="Y26">
+        <v>0</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>0</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+      <c r="J27">
+        <v>1</v>
+      </c>
+      <c r="K27">
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <v>0</v>
+      </c>
+      <c r="M27">
+        <v>0</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>0</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="Q27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>0</v>
+      </c>
+      <c r="T27">
+        <v>0</v>
+      </c>
+      <c r="U27">
+        <v>0</v>
+      </c>
+      <c r="V27">
+        <v>0</v>
+      </c>
+      <c r="W27">
+        <v>0</v>
+      </c>
+      <c r="X27">
+        <v>0</v>
+      </c>
+      <c r="Y27">
+        <v>0</v>
+      </c>
+      <c r="Z27">
+        <v>1</v>
+      </c>
+      <c r="AA27">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CD4AFB0-01E2-7B4F-9AF4-304BF909169C}">
   <dimension ref="A1:B13"/>
   <sheetViews>
@@ -28082,8 +30339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77735C93-7ED9-C044-B61C-E23C86F44D03}">
   <dimension ref="A1:E1763"/>
   <sheetViews>
-    <sheetView topLeftCell="A1714" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="A1738" sqref="A1738:A1763"/>
+    <sheetView topLeftCell="A1731" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="B1738" sqref="B1738:B1763"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added more county data
</commit_message>
<xml_diff>
--- a/shiny/covid19_hamilton/latest_irish_data.xlsx
+++ b/shiny/covid19_hamilton/latest_irish_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/MacintoshHD2/GitHub/covid19ireland/shiny/covid19_hamilton/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B40F6AF4-7138-E240-964B-18D3ABF4D68E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F3556E-672C-2442-B12E-A1467A0DAFD5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="26720" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="updated" sheetId="6" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <sheet name="NI_gender" sheetId="8" r:id="rId10"/>
     <sheet name="NI_age" sheetId="9" r:id="rId11"/>
     <sheet name="NI_district" sheetId="10" r:id="rId12"/>
-    <sheet name="Adjacency_matrix" sheetId="14" r:id="rId13"/>
+    <sheet name="Coiunty" sheetId="14" r:id="rId13"/>
     <sheet name="NI_county_lookup" sheetId="11" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -95,7 +95,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4018" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4020" uniqueCount="223">
   <si>
     <t>Date</t>
   </si>
@@ -762,6 +762,9 @@
   <si>
     <t>https://www.gov.ie/en/press-release/09b5b-statement-from-the-national-public-health-emergency-team-wednesday-27-may/</t>
   </si>
+  <si>
+    <t>Pop_2016</t>
+  </si>
 </sst>
 </file>
 
@@ -1269,7 +1272,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1300,6 +1303,7 @@
     <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -6718,18 +6722,21 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{349ABED6-B9F8-C047-A7E7-BF15BC014788}">
-  <dimension ref="A1:AA27"/>
+  <dimension ref="A1:AB65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
       <c r="B1" t="s">
         <v>12</v>
       </c>
@@ -6808,8 +6815,11 @@
       <c r="AA1" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -6891,8 +6901,11 @@
       <c r="AA2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB2">
+        <v>56932</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
@@ -6974,8 +6987,11 @@
       <c r="AA3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB3">
+        <v>76176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -7057,8 +7073,11 @@
       <c r="AA4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB4">
+        <v>118817</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -7140,8 +7159,11 @@
       <c r="AA5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB5">
+        <v>542868</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -7223,8 +7245,11 @@
       <c r="AA6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB6">
+        <v>159192</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -7306,8 +7331,11 @@
       <c r="AA7">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB7">
+        <v>1347359</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -7389,8 +7417,11 @@
       <c r="AA8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB8">
+        <v>258058</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>20</v>
       </c>
@@ -7472,8 +7503,11 @@
       <c r="AA9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB9">
+        <v>147707</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -7555,8 +7589,11 @@
       <c r="AA10">
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB10">
+        <v>222504</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -7638,8 +7675,11 @@
       <c r="AA11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB11">
+        <v>99232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -7721,8 +7761,11 @@
       <c r="AA12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB12">
+        <v>84697</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -7804,8 +7847,11 @@
       <c r="AA13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB13">
+        <v>32044</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -7887,8 +7933,11 @@
       <c r="AA14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB14">
+        <v>194899</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>24</v>
       </c>
@@ -7970,8 +8019,11 @@
       <c r="AA15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB15">
+        <v>40873</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>25</v>
       </c>
@@ -8053,8 +8105,11 @@
       <c r="AA16">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB16">
+        <v>128884</v>
+      </c>
+    </row>
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>26</v>
       </c>
@@ -8136,8 +8191,11 @@
       <c r="AA17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB17">
+        <v>130507</v>
+      </c>
+    </row>
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>27</v>
       </c>
@@ -8219,8 +8277,11 @@
       <c r="AA18">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB18">
+        <v>195044</v>
+      </c>
+    </row>
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -8302,8 +8363,11 @@
       <c r="AA19">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB19">
+        <v>61386</v>
+      </c>
+    </row>
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>28</v>
       </c>
@@ -8385,8 +8449,11 @@
       <c r="AA20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB20">
+        <v>77961</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>29</v>
       </c>
@@ -8468,8 +8535,11 @@
       <c r="AA21">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB21">
+        <v>64544</v>
+      </c>
+    </row>
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>30</v>
       </c>
@@ -8551,8 +8621,11 @@
       <c r="AA22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB22">
+        <v>65535</v>
+      </c>
+    </row>
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>31</v>
       </c>
@@ -8634,8 +8707,11 @@
       <c r="AA23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB23">
+        <v>159553</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>32</v>
       </c>
@@ -8717,8 +8793,11 @@
       <c r="AA24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB24">
+        <v>116176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>33</v>
       </c>
@@ -8800,8 +8879,11 @@
       <c r="AA25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB25">
+        <v>88770</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>34</v>
       </c>
@@ -8883,8 +8965,11 @@
       <c r="AA26">
         <v>1</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AB26">
+        <v>149722</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>35</v>
       </c>
@@ -8966,6 +9051,149 @@
       <c r="AA27">
         <v>0</v>
       </c>
+      <c r="AB27">
+        <v>142425</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="U31" s="15"/>
+      <c r="X31" s="3"/>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="U32" s="15"/>
+      <c r="X32" s="3"/>
+    </row>
+    <row r="33" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U33" s="15"/>
+      <c r="X33" s="3"/>
+    </row>
+    <row r="34" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U34" s="15"/>
+      <c r="X34" s="3"/>
+    </row>
+    <row r="35" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U35" s="15"/>
+      <c r="X35" s="3"/>
+    </row>
+    <row r="36" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U36" s="15"/>
+      <c r="X36" s="3"/>
+    </row>
+    <row r="37" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U37" s="15"/>
+    </row>
+    <row r="38" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U38" s="15"/>
+      <c r="X38" s="3"/>
+    </row>
+    <row r="39" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U39" s="15"/>
+      <c r="V39" s="20"/>
+      <c r="X39" s="3"/>
+    </row>
+    <row r="40" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U40" s="15"/>
+      <c r="V40" s="20"/>
+      <c r="X40" s="3"/>
+    </row>
+    <row r="41" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U41" s="15"/>
+      <c r="X41" s="3"/>
+    </row>
+    <row r="42" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U42" s="15"/>
+      <c r="X42" s="3"/>
+    </row>
+    <row r="43" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U43" s="15"/>
+      <c r="X43" s="3"/>
+    </row>
+    <row r="44" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U44" s="15"/>
+      <c r="X44" s="3"/>
+    </row>
+    <row r="45" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U45" s="15"/>
+      <c r="X45" s="3"/>
+    </row>
+    <row r="46" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U46" s="15"/>
+      <c r="X46" s="3"/>
+    </row>
+    <row r="47" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U47" s="15"/>
+      <c r="X47" s="3"/>
+    </row>
+    <row r="48" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U48" s="15"/>
+      <c r="X48" s="3"/>
+    </row>
+    <row r="49" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U49" s="15"/>
+      <c r="X49" s="3"/>
+    </row>
+    <row r="50" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U50" s="15"/>
+      <c r="X50" s="3"/>
+    </row>
+    <row r="51" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U51" s="15"/>
+      <c r="X51" s="3"/>
+    </row>
+    <row r="52" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U52" s="15"/>
+      <c r="X52" s="3"/>
+    </row>
+    <row r="53" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U53" s="15"/>
+    </row>
+    <row r="54" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U54" s="15"/>
+      <c r="X54" s="3"/>
+    </row>
+    <row r="55" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U55" s="15"/>
+      <c r="X55" s="3"/>
+    </row>
+    <row r="56" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U56" s="15"/>
+      <c r="X56" s="3"/>
+    </row>
+    <row r="57" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U57" s="15"/>
+      <c r="X57" s="3"/>
+    </row>
+    <row r="58" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U58" s="15"/>
+    </row>
+    <row r="59" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U59" s="15"/>
+      <c r="V59" s="20"/>
+      <c r="X59" s="3"/>
+    </row>
+    <row r="60" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U60" s="15"/>
+      <c r="X60" s="3"/>
+    </row>
+    <row r="61" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U61" s="15"/>
+      <c r="X61" s="3"/>
+    </row>
+    <row r="62" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U62" s="15"/>
+      <c r="X62" s="3"/>
+    </row>
+    <row r="63" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U63" s="15"/>
+      <c r="X63" s="3"/>
+    </row>
+    <row r="64" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U64" s="15"/>
+      <c r="X64" s="3"/>
+    </row>
+    <row r="65" spans="21:24" x14ac:dyDescent="0.2">
+      <c r="U65" s="15"/>
+      <c r="X65" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>